<commit_message>
Contest 1 MI vs RCB
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CE5A9D-F320-0A43-B5F5-6DE3E842DD4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD60698-8EAF-0D43-A80F-ECDC7C913FF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="460" windowWidth="30120" windowHeight="20620" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="1360" yWindow="4280" windowWidth="29480" windowHeight="16740" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="56">
   <si>
     <t>Points</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Sampath M</t>
   </si>
   <si>
-    <t>MI vs CSK</t>
-  </si>
-  <si>
     <t>Prize</t>
   </si>
   <si>
@@ -158,6 +155,51 @@
   </si>
   <si>
     <t>Finals MI vs DC</t>
+  </si>
+  <si>
+    <t>MI vs RCB</t>
+  </si>
+  <si>
+    <t>CSK vs DC</t>
+  </si>
+  <si>
+    <t>SRH vs KKR</t>
+  </si>
+  <si>
+    <t>RR vs PBKS</t>
+  </si>
+  <si>
+    <t>KKR vs MI</t>
+  </si>
+  <si>
+    <t>SRH vs RCB</t>
+  </si>
+  <si>
+    <t>RR vs DC</t>
+  </si>
+  <si>
+    <t>PBKS vs CSK</t>
+  </si>
+  <si>
+    <t>MI vs SRH</t>
+  </si>
+  <si>
+    <t>RCB vs KKR</t>
+  </si>
+  <si>
+    <t>DC vs PBKS</t>
+  </si>
+  <si>
+    <t>CSK vs RR</t>
+  </si>
+  <si>
+    <t>DC vs MI</t>
+  </si>
+  <si>
+    <t>PBKS vs SRH</t>
+  </si>
+  <si>
+    <t>KKR vs CSK</t>
   </si>
 </sst>
 </file>
@@ -428,7 +470,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -943,7 +985,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -957,7 +999,7 @@
         <v>50</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
@@ -1036,27 +1078,27 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D8" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="20"/>
       <c r="G8" s="20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="20"/>
       <c r="J8" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K8" s="20"/>
       <c r="M8" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N8" s="20"/>
       <c r="P8" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q8" s="20"/>
       <c r="S8" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T8" s="20"/>
     </row>
@@ -1115,14 +1157,14 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D10" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E10, ($T10,$Q10,$N10,$K10,$H10,$E10), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E10, ($T10,$Q10,$N10,$K10,$H10,$E10), 0),  score, 2, FALSE))</f>
-        <v>-15</v>
+        <v>-20</v>
       </c>
       <c r="E10" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="G10" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H10, ($T10,$Q10,$N10,$K10,$H10,$E10), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H10, ($T10,$Q10,$N10,$K10,$H10,$E10), 0),  score, 2, FALSE))</f>
@@ -1133,10 +1175,10 @@
       </c>
       <c r="J10" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K10, ($T10,$Q10,$N10,$K10,$H10,$E10), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K10, ($T10,$Q10,$N10,$K10,$H10,$E10), 0),  score, 2, FALSE))</f>
-        <v>-10</v>
+        <v>-25</v>
       </c>
       <c r="K10" s="1">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="M10" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N10, ($T10,$Q10,$N10,$K10,$H10,$E10), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N10, ($T10,$Q10,$N10,$K10,$H10,$E10), 0),  score, 2, FALSE))</f>
@@ -1147,17 +1189,17 @@
       </c>
       <c r="P10" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q10, ($T10,$Q10,$N10,$K10,$H10,$E10), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q10, ($T10,$Q10,$N10,$K10,$H10,$E10), 0),  score, 2, FALSE))</f>
-        <v>-20</v>
+        <v>-10</v>
       </c>
       <c r="Q10" s="1">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="S10" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T10, ($T10,$Q10,$N10,$K10,$H10,$E10), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T10, ($T10,$Q10,$N10,$K10,$H10,$E10), 0),  score, 2, FALSE))</f>
-        <v>-25</v>
+        <v>-15</v>
       </c>
       <c r="T10" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -1167,7 +1209,9 @@
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="D11" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1206,7 +1250,9 @@
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="D12" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1245,7 +1291,9 @@
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="D13" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1284,7 +1332,9 @@
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="D14" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1323,7 +1373,9 @@
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="D15" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1362,7 +1414,9 @@
       <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="23"/>
+      <c r="C16" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D16" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1401,7 +1455,9 @@
       <c r="B17" s="1">
         <v>1</v>
       </c>
-      <c r="C17" s="23"/>
+      <c r="C17" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="D17" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1440,7 +1496,9 @@
       <c r="B18" s="1">
         <v>1</v>
       </c>
-      <c r="C18" s="23"/>
+      <c r="C18" s="23" t="s">
+        <v>49</v>
+      </c>
       <c r="D18" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1479,7 +1537,9 @@
       <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="23"/>
+      <c r="C19" s="23" t="s">
+        <v>50</v>
+      </c>
       <c r="D19" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1518,7 +1578,9 @@
       <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C20" s="23"/>
+      <c r="C20" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="D20" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1557,7 +1619,9 @@
       <c r="B21" s="1">
         <v>1</v>
       </c>
-      <c r="C21" s="23"/>
+      <c r="C21" s="23" t="s">
+        <v>52</v>
+      </c>
       <c r="D21" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1596,7 +1660,9 @@
       <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C22" s="23"/>
+      <c r="C22" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="D22" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1635,7 +1701,9 @@
       <c r="B23" s="1">
         <v>1</v>
       </c>
-      <c r="C23" s="23"/>
+      <c r="C23" s="23" t="s">
+        <v>54</v>
+      </c>
       <c r="D23" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1674,7 +1742,9 @@
       <c r="B24" s="1">
         <v>1</v>
       </c>
-      <c r="C24" s="23"/>
+      <c r="C24" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="D24" s="3" t="str">
         <f>IF(ISERROR(VLOOKUP(RANK(E24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
         <v/>
@@ -1714,27 +1784,27 @@
       <c r="C25" s="9"/>
       <c r="D25" s="1"/>
       <c r="E25" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M25" s="1"/>
       <c r="N25" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S25" s="1"/>
       <c r="T25" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
@@ -1777,46 +1847,46 @@
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E27" s="11">
         <f>SUM(D10:D14)</f>
-        <v>-15</v>
+        <v>-20</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H27" s="11">
         <f>SUM(G10:G14)</f>
         <v>20</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K27" s="11">
         <f>SUM(J10:J14)</f>
-        <v>-10</v>
+        <v>-25</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N27" s="11">
         <f>SUM(M10:M14)</f>
         <v>50</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q27" s="11">
         <f>SUM(P10:P14)</f>
-        <v>-20</v>
+        <v>-10</v>
       </c>
       <c r="S27" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T27" s="11">
         <f>SUM(S10:S14)</f>
-        <v>-25</v>
+        <v>-15</v>
       </c>
       <c r="U27" s="1">
         <f>SUM(E27,H27,K27,N27,Q27,T27)</f>
@@ -1943,67 +2013,67 @@
   <sheetData>
     <row r="17" spans="6:10" ht="24" x14ac:dyDescent="0.3">
       <c r="I17" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="6:10" ht="24" x14ac:dyDescent="0.3">
       <c r="I18" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="6:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I19" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="6:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I20" s="22"/>
       <c r="J20" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="6:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I21" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="6:10" ht="24" x14ac:dyDescent="0.3">
       <c r="I22" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="6:10" ht="24" x14ac:dyDescent="0.3">
       <c r="I23" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="28" spans="6:10" x14ac:dyDescent="0.2">
@@ -2074,13 +2144,13 @@
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F36" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G36" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H36" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.2">
@@ -2146,18 +2216,18 @@
         <v>8</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F45" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G45" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H45" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="46" spans="6:8" x14ac:dyDescent="0.2">
@@ -2165,7 +2235,7 @@
         <v>5</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H46" s="17" t="s">
         <v>6</v>
@@ -2228,13 +2298,13 @@
     </row>
     <row r="54" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F54" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G54" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H54" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="55" spans="6:8" x14ac:dyDescent="0.2">
@@ -2289,7 +2359,7 @@
         <v>8</v>
       </c>
       <c r="H59" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" spans="6:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Contest 4 RR vs PBKS
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD60698-8EAF-0D43-A80F-ECDC7C913FF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A851FA01-AC4E-F54B-811B-EDC8266A6C68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="4280" windowWidth="29480" windowHeight="16740" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -1212,36 +1212,48 @@
       <c r="C11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="3" t="str">
+      <c r="D11" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="G11" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E11" s="1">
+        <v>20</v>
+      </c>
+      <c r="G11" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="J11" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1">
+        <v>80</v>
+      </c>
+      <c r="J11" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="M11" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K11" s="1">
+        <v>40</v>
+      </c>
+      <c r="M11" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N11" s="1"/>
-      <c r="P11" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q11" s="1"/>
-      <c r="S11" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>100</v>
+      </c>
+      <c r="S11" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T11, ($T11,$Q11,$N11,$K11,$H11,$E11), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T11" s="1"/>
+        <v>-10</v>
+      </c>
+      <c r="T11" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1253,36 +1265,48 @@
       <c r="C12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="3" t="str">
+      <c r="D12" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="G12" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E12" s="1">
+        <v>60</v>
+      </c>
+      <c r="G12" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="J12" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H12" s="1">
+        <v>20</v>
+      </c>
+      <c r="J12" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="M12" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K12" s="1">
+        <v>80</v>
+      </c>
+      <c r="M12" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N12" s="1"/>
-      <c r="P12" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N12" s="1">
+        <v>100</v>
+      </c>
+      <c r="P12" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q12" s="1"/>
-      <c r="S12" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>40</v>
+      </c>
+      <c r="S12" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T12, ($T12,$Q12,$N12,$K12,$H12,$E12), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T12" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1294,36 +1318,48 @@
       <c r="C13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="3" t="str">
+      <c r="D13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="G13" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E13" s="1">
+        <v>100</v>
+      </c>
+      <c r="G13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="J13" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H13" s="1">
+        <v>60</v>
+      </c>
+      <c r="J13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K13" s="1"/>
-      <c r="M13" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N13" s="1"/>
-      <c r="P13" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N13" s="1">
+        <v>20</v>
+      </c>
+      <c r="P13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q13" s="1"/>
-      <c r="S13" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>80</v>
+      </c>
+      <c r="S13" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T13, ($T13,$Q13,$N13,$K13,$H13,$E13), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T13" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="T13" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1851,42 +1887,42 @@
       </c>
       <c r="E27" s="11">
         <f>SUM(D10:D14)</f>
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="11">
         <f>SUM(G10:G14)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K27" s="11">
         <f>SUM(J10:J14)</f>
-        <v>-25</v>
+        <v>-45</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N27" s="11">
         <f>SUM(M10:M14)</f>
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q27" s="11">
         <f>SUM(P10:P14)</f>
-        <v>-10</v>
+        <v>45</v>
       </c>
       <c r="S27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T27" s="11">
         <f>SUM(S10:S14)</f>
-        <v>-15</v>
+        <v>-65</v>
       </c>
       <c r="U27" s="1">
         <f>SUM(E27,H27,K27,N27,Q27,T27)</f>

</xml_diff>

<commit_message>
contest 7 SRH vs RR.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A851FA01-AC4E-F54B-811B-EDC8266A6C68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154AF16F-4402-1B4D-B10B-526F1EB9E126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="4280" windowWidth="29480" windowHeight="16740" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -458,6 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -470,7 +471,6 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -478,7 +478,157 @@
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -998,15 +1148,15 @@
       <c r="B2" s="7">
         <v>50</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
@@ -1015,13 +1165,13 @@
       <c r="B3" s="7">
         <v>20</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
@@ -1030,13 +1180,13 @@
       <c r="B4" s="7">
         <v>-10</v>
       </c>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
@@ -1045,13 +1195,13 @@
       <c r="B5" s="7">
         <v>-15</v>
       </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
@@ -1060,13 +1210,13 @@
       <c r="B6" s="7">
         <v>-20</v>
       </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
@@ -1077,30 +1227,30 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="G8" s="20" t="s">
+      <c r="E8" s="21"/>
+      <c r="G8" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="J8" s="20" t="s">
+      <c r="H8" s="21"/>
+      <c r="J8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="20"/>
-      <c r="M8" s="20" t="s">
+      <c r="K8" s="21"/>
+      <c r="M8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="20"/>
-      <c r="P8" s="20" t="s">
+      <c r="N8" s="21"/>
+      <c r="P8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="Q8" s="20"/>
-      <c r="S8" s="20" t="s">
+      <c r="Q8" s="21"/>
+      <c r="S8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="T8" s="20"/>
+      <c r="T8" s="21"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
@@ -1371,36 +1521,46 @@
       <c r="C14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="G14" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="J14" s="3" t="str">
+      <c r="D14" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="E14" s="1">
+        <v>20</v>
+      </c>
+      <c r="G14" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="H14" s="1">
+        <v>20</v>
+      </c>
+      <c r="J14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="M14" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K14" s="1">
+        <v>60</v>
+      </c>
+      <c r="M14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N14" s="1"/>
-      <c r="P14" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N14" s="1">
+        <v>80</v>
+      </c>
+      <c r="P14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q14" s="1"/>
-      <c r="S14" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>100</v>
+      </c>
+      <c r="S14" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T14, ($T14,$Q14,$N14,$K14,$H14,$E14), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T14" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="T14" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1412,36 +1572,48 @@
       <c r="C15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="3" t="str">
+      <c r="D15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="G15" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E15" s="1">
+        <v>80</v>
+      </c>
+      <c r="G15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="J15" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H15" s="1">
+        <v>20</v>
+      </c>
+      <c r="J15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="M15" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K15" s="1">
+        <v>40</v>
+      </c>
+      <c r="M15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N15" s="1"/>
-      <c r="P15" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N15" s="1">
+        <v>100</v>
+      </c>
+      <c r="P15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q15" s="1"/>
-      <c r="S15" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>60</v>
+      </c>
+      <c r="S15" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T15, ($T15,$Q15,$N15,$K15,$H15,$E15), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T15" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T15" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1532,7 +1704,7 @@
       <c r="B18" s="1">
         <v>1</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D18" s="3" t="str">
@@ -1573,7 +1745,7 @@
       <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="19" t="s">
         <v>50</v>
       </c>
       <c r="D19" s="3" t="str">
@@ -1614,7 +1786,7 @@
       <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="19" t="s">
         <v>51</v>
       </c>
       <c r="D20" s="3" t="str">
@@ -1655,7 +1827,7 @@
       <c r="B21" s="1">
         <v>1</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="19" t="s">
         <v>52</v>
       </c>
       <c r="D21" s="3" t="str">
@@ -1696,7 +1868,7 @@
       <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="19" t="s">
         <v>53</v>
       </c>
       <c r="D22" s="3" t="str">
@@ -1737,7 +1909,7 @@
       <c r="B23" s="1">
         <v>1</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="19" t="s">
         <v>54</v>
       </c>
       <c r="D23" s="3" t="str">
@@ -1778,7 +1950,7 @@
       <c r="B24" s="1">
         <v>1</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="19" t="s">
         <v>55</v>
       </c>
       <c r="D24" s="3" t="str">
@@ -1886,43 +2058,43 @@
         <v>12</v>
       </c>
       <c r="E27" s="11">
-        <f>SUM(D10:D14)</f>
-        <v>0</v>
+        <f>SUM(D10:D24)</f>
+        <v>-2.5</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="11">
-        <f>SUM(G10:G14)</f>
-        <v>10</v>
+        <f>SUM(G10:G24)</f>
+        <v>-32.5</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K27" s="11">
-        <f>SUM(J10:J14)</f>
-        <v>-45</v>
+        <f>SUM(J10:J24)</f>
+        <v>-70</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N27" s="11">
-        <f>SUM(M10:M14)</f>
-        <v>55</v>
+        <f>SUM(M10:M24)</f>
+        <v>125</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q27" s="11">
-        <f>SUM(P10:P14)</f>
-        <v>45</v>
+        <f>SUM(P10:P24)</f>
+        <v>85</v>
       </c>
       <c r="S27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T27" s="11">
-        <f>SUM(S10:S14)</f>
-        <v>-65</v>
+        <f>SUM(S10:S24)</f>
+        <v>-105</v>
       </c>
       <c r="U27" s="1">
         <f>SUM(E27,H27,K27,N27,Q27,T27)</f>
@@ -1961,68 +2133,68 @@
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
   <conditionalFormatting sqref="E27">
-    <cfRule type="cellIs" dxfId="17" priority="61" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="76" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="77" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="63" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="78" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27">
-    <cfRule type="cellIs" dxfId="14" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="27" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="11" priority="28" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="29" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27">
-    <cfRule type="cellIs" dxfId="8" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q27">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T27">
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q27">
-    <cfRule type="cellIs" dxfId="2" priority="16" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="17" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2064,7 +2236,7 @@
       </c>
     </row>
     <row r="19" spans="6:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I19" s="21" t="s">
+      <c r="I19" s="22" t="s">
         <v>23</v>
       </c>
       <c r="J19" s="13" t="s">
@@ -2072,7 +2244,7 @@
       </c>
     </row>
     <row r="20" spans="6:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I20" s="22"/>
+      <c r="I20" s="23"/>
       <c r="J20" s="13" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
contest 7 RR vs DC
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955E3001-6882-C54A-ABE8-4E9324C7C89C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7378ED6B-7FDF-0A4E-8C27-F54F7FEFB347}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="4280" windowWidth="29480" windowHeight="16740" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -1625,36 +1625,48 @@
       <c r="C16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="3" t="str">
+      <c r="D16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="G16" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E16" s="1">
+        <v>80</v>
+      </c>
+      <c r="G16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="J16" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H16" s="1">
+        <v>40</v>
+      </c>
+      <c r="J16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="M16" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K16" s="1">
+        <v>20</v>
+      </c>
+      <c r="M16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N16" s="1"/>
-      <c r="P16" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N16" s="1">
+        <v>60</v>
+      </c>
+      <c r="P16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q16" s="1"/>
-      <c r="S16" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0</v>
+      </c>
+      <c r="S16" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T16, ($T16,$Q16,$N16,$K16,$H16,$E16), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T16" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="T16" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -2059,42 +2071,42 @@
       </c>
       <c r="E27" s="11">
         <f>SUM(D10:D24)</f>
-        <v>-2.5</v>
+        <v>17.5</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="11">
         <f>SUM(G10:G24)</f>
-        <v>-32.5</v>
+        <v>-47.5</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K27" s="11">
         <f>SUM(J10:J24)</f>
-        <v>-70</v>
+        <v>-90</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N27" s="11">
         <f>SUM(M10:M24)</f>
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q27" s="11">
         <f>SUM(P10:P24)</f>
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="S27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T27" s="11">
         <f>SUM(S10:S24)</f>
-        <v>-105</v>
+        <v>-55</v>
       </c>
       <c r="U27" s="1">
         <f>SUM(E27,H27,K27,N27,Q27,T27)</f>

</xml_diff>

<commit_message>
Contest 8 PBKS vs CSK
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7378ED6B-7FDF-0A4E-8C27-F54F7FEFB347}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4241CC97-F862-434F-AC0B-D076A4BE72A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="4280" windowWidth="29480" windowHeight="16740" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="880" yWindow="4340" windowWidth="30080" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1678,36 +1678,48 @@
       <c r="C17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="3" t="str">
+      <c r="D17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="G17" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="E17" s="1">
+        <v>80</v>
+      </c>
+      <c r="G17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="J17" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H17" s="1">
+        <v>20</v>
+      </c>
+      <c r="J17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K17" s="1"/>
-      <c r="M17" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K17" s="1">
+        <v>100</v>
+      </c>
+      <c r="M17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N17" s="1"/>
-      <c r="P17" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="P17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q17" s="1"/>
-      <c r="S17" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>40</v>
+      </c>
+      <c r="S17" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T17, ($T17,$Q17,$N17,$K17,$H17,$E17), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T17" s="1"/>
+        <v>-10</v>
+      </c>
+      <c r="T17" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -2071,42 +2083,42 @@
       </c>
       <c r="E27" s="11">
         <f>SUM(D10:D24)</f>
-        <v>17.5</v>
+        <v>37.5</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="11">
         <f>SUM(G10:G24)</f>
-        <v>-47.5</v>
+        <v>-67.5</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K27" s="11">
         <f>SUM(J10:J24)</f>
-        <v>-90</v>
+        <v>-40</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N27" s="11">
         <f>SUM(M10:M24)</f>
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q27" s="11">
         <f>SUM(P10:P24)</f>
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="S27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T27" s="11">
         <f>SUM(S10:S24)</f>
-        <v>-55</v>
+        <v>-65</v>
       </c>
       <c r="U27" s="1">
         <f>SUM(E27,H27,K27,N27,Q27,T27)</f>

</xml_diff>

<commit_message>
Contest 10 and 11 RCB vs KKR and DC vs PBKS
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4241CC97-F862-434F-AC0B-D076A4BE72A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15BB77A-B37B-414E-9677-081AA2B0CCAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="4340" windowWidth="30080" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -1731,36 +1731,48 @@
       <c r="C18" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="3" t="str">
+      <c r="D18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="G18" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E18" s="1">
+        <v>40</v>
+      </c>
+      <c r="G18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H18" s="1"/>
-      <c r="J18" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H18" s="1">
+        <v>20</v>
+      </c>
+      <c r="J18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K18" s="1"/>
-      <c r="M18" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K18" s="1">
+        <v>100</v>
+      </c>
+      <c r="M18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N18" s="1"/>
-      <c r="P18" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N18" s="1">
+        <v>60</v>
+      </c>
+      <c r="P18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q18" s="1"/>
-      <c r="S18" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>80</v>
+      </c>
+      <c r="S18" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T18, ($T18,$Q18,$N18,$K18,$H18,$E18), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T18" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T18" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1772,36 +1784,48 @@
       <c r="C19" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="3" t="str">
+      <c r="D19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="G19" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="J19" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H19" s="1">
+        <v>40</v>
+      </c>
+      <c r="J19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K19" s="1"/>
-      <c r="M19" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K19" s="1">
+        <v>20</v>
+      </c>
+      <c r="M19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N19" s="1"/>
-      <c r="P19" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N19" s="1">
+        <v>60</v>
+      </c>
+      <c r="P19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q19" s="1"/>
-      <c r="S19" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>80</v>
+      </c>
+      <c r="S19" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T19, ($T19,$Q19,$N19,$K19,$H19,$E19), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T19" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="T19" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1813,36 +1837,48 @@
       <c r="C20" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="3" t="str">
+      <c r="D20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="G20" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E20" s="1">
+        <v>60</v>
+      </c>
+      <c r="G20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="J20" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H20" s="1">
+        <v>100</v>
+      </c>
+      <c r="J20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K20" s="1"/>
-      <c r="M20" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K20" s="1">
+        <v>20</v>
+      </c>
+      <c r="M20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N20" s="1"/>
-      <c r="P20" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q20" s="1"/>
-      <c r="S20" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>40</v>
+      </c>
+      <c r="S20" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T20, ($T20,$Q20,$N20,$K20,$H20,$E20), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T20" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="T20" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -2083,42 +2119,42 @@
       </c>
       <c r="E27" s="11">
         <f>SUM(D10:D24)</f>
-        <v>37.5</v>
+        <v>-12.5</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="11">
         <f>SUM(G10:G24)</f>
-        <v>-67.5</v>
+        <v>-52.5</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K27" s="11">
         <f>SUM(J10:J24)</f>
-        <v>-40</v>
+        <v>-30</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N27" s="11">
         <f>SUM(M10:M24)</f>
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q27" s="11">
         <f>SUM(P10:P24)</f>
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="S27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T27" s="11">
         <f>SUM(S10:S24)</f>
-        <v>-65</v>
+        <v>-20</v>
       </c>
       <c r="U27" s="1">
         <f>SUM(E27,H27,K27,N27,Q27,T27)</f>

</xml_diff>

<commit_message>
Contest 12 CSK vs RR
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15BB77A-B37B-414E-9677-081AA2B0CCAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E0DD32-E665-3948-A487-41245E4D8AB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="4340" windowWidth="30080" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -1890,36 +1890,48 @@
       <c r="C21" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="3" t="str">
+      <c r="D21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="G21" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E21" s="1">
+        <v>100</v>
+      </c>
+      <c r="G21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="J21" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1">
+        <v>80</v>
+      </c>
+      <c r="J21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K21" s="1"/>
-      <c r="M21" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K21" s="1">
+        <v>20</v>
+      </c>
+      <c r="M21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N21" s="1"/>
-      <c r="P21" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q21" s="1"/>
-      <c r="S21" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>60</v>
+      </c>
+      <c r="S21" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T21" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="T21" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -2119,42 +2131,42 @@
       </c>
       <c r="E27" s="11">
         <f>SUM(D10:D24)</f>
-        <v>-12.5</v>
+        <v>37.5</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H27" s="11">
         <f>SUM(G10:G24)</f>
-        <v>-52.5</v>
+        <v>-32.5</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K27" s="11">
         <f>SUM(J10:J24)</f>
-        <v>-30</v>
+        <v>-50</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N27" s="11">
         <f>SUM(M10:M24)</f>
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q27" s="11">
         <f>SUM(P10:P24)</f>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="S27" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T27" s="11">
         <f>SUM(S10:S24)</f>
-        <v>-20</v>
+        <v>-35</v>
       </c>
       <c r="U27" s="1">
         <f>SUM(E27,H27,K27,N27,Q27,T27)</f>

</xml_diff>

<commit_message>
Contest 15 KKR vs CSK. Added 15 more contests.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E0DD32-E665-3948-A487-41245E4D8AB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230DC6FC-403F-AF46-AB54-9AE0211F3CE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="4340" windowWidth="30080" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="1440" yWindow="4400" windowWidth="22700" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="72">
   <si>
     <t>Points</t>
   </si>
@@ -200,6 +200,54 @@
   </si>
   <si>
     <t>KKR vs CSK</t>
+  </si>
+  <si>
+    <t>Fromat 2</t>
+  </si>
+  <si>
+    <t>RCB vs RR</t>
+  </si>
+  <si>
+    <t>PBKS vs MI</t>
+  </si>
+  <si>
+    <t>RR vs KKR</t>
+  </si>
+  <si>
+    <t>CSK vs RCB</t>
+  </si>
+  <si>
+    <t>SRH vs DC</t>
+  </si>
+  <si>
+    <t>PBKS vs KKR</t>
+  </si>
+  <si>
+    <t>DC vs RCB</t>
+  </si>
+  <si>
+    <t>CSK vs SRH</t>
+  </si>
+  <si>
+    <t>MI vs RR</t>
+  </si>
+  <si>
+    <t>DC vs KKR</t>
+  </si>
+  <si>
+    <t>PBKS vs RCB</t>
+  </si>
+  <si>
+    <t>MI vs CSK</t>
+  </si>
+  <si>
+    <t>RR vs SRH</t>
+  </si>
+  <si>
+    <t>PBKS vs DC</t>
+  </si>
+  <si>
+    <t>KKR vs RCB</t>
   </si>
 </sst>
 </file>
@@ -428,7 +476,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -471,6 +519,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -1119,11 +1168,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U30"/>
+  <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U27" sqref="U27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1140,6 +1189,9 @@
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
@@ -1147,6 +1199,9 @@
       </c>
       <c r="B2" s="7">
         <v>50</v>
+      </c>
+      <c r="C2" s="7">
+        <v>40</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>20</v>
@@ -1164,6 +1219,9 @@
       </c>
       <c r="B3" s="7">
         <v>20</v>
+      </c>
+      <c r="C3" s="7">
+        <v>15</v>
       </c>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
@@ -1180,6 +1238,9 @@
       <c r="B4" s="7">
         <v>-10</v>
       </c>
+      <c r="C4" s="7">
+        <v>-10</v>
+      </c>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
@@ -1195,6 +1256,9 @@
       <c r="B5" s="7">
         <v>-15</v>
       </c>
+      <c r="C5" s="7">
+        <v>-20</v>
+      </c>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
@@ -1210,6 +1274,9 @@
       <c r="B6" s="7">
         <v>-20</v>
       </c>
+      <c r="C6" s="7">
+        <v>-25</v>
+      </c>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
@@ -1225,6 +1292,9 @@
       <c r="B7" s="7">
         <v>-25</v>
       </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D8" s="21" t="s">
@@ -1668,7 +1738,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>8</v>
       </c>
@@ -1721,7 +1791,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -1774,7 +1844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>10</v>
       </c>
@@ -1827,7 +1897,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>11</v>
       </c>
@@ -1880,142 +1950,166 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>12</v>
       </c>
       <c r="B21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>52</v>
       </c>
       <c r="D21" s="3">
-        <f>IF(ISERROR(VLOOKUP(RANK(E21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v>50</v>
+        <f>IF(ISERROR(VLOOKUP(RANK(E21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$C$7, $B21+1, FALSE)),"",VLOOKUP(RANK(E21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$C$7, $B21+1, FALSE))</f>
+        <v>40</v>
       </c>
       <c r="E21" s="1">
         <v>100</v>
       </c>
       <c r="G21" s="3">
-        <f>IF(ISERROR(VLOOKUP(RANK(H21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v>20</v>
+        <f>IF(ISERROR(VLOOKUP(RANK(H21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$C$7, $B21+1, FALSE)),"",VLOOKUP(RANK(H21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$C$7, $B21+1, FALSE))</f>
+        <v>15</v>
       </c>
       <c r="H21" s="1">
         <v>80</v>
       </c>
       <c r="J21" s="3">
-        <f>IF(ISERROR(VLOOKUP(RANK(K21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v>-20</v>
+        <f>IF(ISERROR(VLOOKUP(RANK(K21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$C$7, $B21+1, FALSE)),"",VLOOKUP(RANK(K21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$C$7, $B21+1, FALSE))</f>
+        <v>-25</v>
       </c>
       <c r="K21" s="1">
         <v>20</v>
       </c>
       <c r="M21" s="3">
-        <f>IF(ISERROR(VLOOKUP(RANK(N21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v>-25</v>
+        <f>IF(ISERROR(VLOOKUP(RANK(N21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$C$7, $B21+1, FALSE)),"",VLOOKUP(RANK(N21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$C$7, $B21+1, FALSE))</f>
+        <v>0</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
       </c>
       <c r="P21" s="3">
-        <f>IF(ISERROR(VLOOKUP(RANK(Q21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
+        <f>IF(ISERROR(VLOOKUP(RANK(Q21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$C$7, $B21+1, FALSE)),"",VLOOKUP(RANK(Q21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$C$7, $B21+1, FALSE))</f>
         <v>-10</v>
       </c>
       <c r="Q21" s="1">
         <v>60</v>
       </c>
       <c r="S21" s="3">
-        <f>IF(ISERROR(VLOOKUP(RANK(T21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  score, 2, FALSE))</f>
-        <v>-15</v>
+        <f>IF(ISERROR(VLOOKUP(RANK(T21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$C$7, $B21+1, FALSE)),"",VLOOKUP(RANK(T21, ($T21,$Q21,$N21,$K21,$H21,$E21), 0),  $A$2:$C$7, $B21+1, FALSE))</f>
+        <v>-20</v>
       </c>
       <c r="T21" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>13</v>
       </c>
       <c r="B22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="G22" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H22" s="1"/>
-      <c r="J22" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K22" s="1"/>
-      <c r="M22" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N22" s="1"/>
-      <c r="P22" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Q22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q22" s="1"/>
-      <c r="S22" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T22" s="1"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D22" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$C$7, $B22+1, FALSE)),"",VLOOKUP(RANK(E22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$C$7, $B22+1, FALSE))</f>
+        <v>15</v>
+      </c>
+      <c r="E22" s="1">
+        <v>80</v>
+      </c>
+      <c r="G22" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$C$7, $B22+1, FALSE)),"",VLOOKUP(RANK(H22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$C$7, $B22+1, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="H22" s="1">
+        <v>20</v>
+      </c>
+      <c r="J22" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$C$7, $B22+1, FALSE)),"",VLOOKUP(RANK(K22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$C$7, $B22+1, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="K22" s="1">
+        <v>60</v>
+      </c>
+      <c r="M22" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$C$7, $B22+1, FALSE)),"",VLOOKUP(RANK(N22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$C$7, $B22+1, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="P22" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$C$7, $B22+1, FALSE)),"",VLOOKUP(RANK(Q22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$C$7, $B22+1, FALSE))</f>
+        <v>40</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>100</v>
+      </c>
+      <c r="S22" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$C$7, $B22+1, FALSE)),"",VLOOKUP(RANK(T22, ($T22,$Q22,$N22,$K22,$H22,$E22), 0),  $A$2:$C$7, $B22+1, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="T22" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>14</v>
       </c>
       <c r="B23" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="G23" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H23" s="1"/>
-      <c r="J23" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K23" s="1"/>
-      <c r="M23" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N23" s="1"/>
-      <c r="P23" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Q23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q23" s="1"/>
-      <c r="S23" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T23" s="1"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="D23" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE)),"",VLOOKUP(RANK(E23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="E23" s="1">
+        <v>20</v>
+      </c>
+      <c r="G23" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE)),"",VLOOKUP(RANK(H23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="H23" s="1">
+        <v>40</v>
+      </c>
+      <c r="J23" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE)),"",VLOOKUP(RANK(K23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE))</f>
+        <v>40</v>
+      </c>
+      <c r="K23" s="1">
+        <v>100</v>
+      </c>
+      <c r="M23" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE)),"",VLOOKUP(RANK(N23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="P23" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE)),"",VLOOKUP(RANK(Q23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>60</v>
+      </c>
+      <c r="S23" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE)),"",VLOOKUP(RANK(T23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE))</f>
+        <v>15</v>
+      </c>
+      <c r="T23" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>15</v>
       </c>
@@ -2025,174 +2119,798 @@
       <c r="C24" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(E24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="G24" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(H24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="J24" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(K24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K24" s="1"/>
-      <c r="M24" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(N24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N24" s="1"/>
-      <c r="P24" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Q24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(Q24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q24" s="1"/>
-      <c r="S24" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE)),"",VLOOKUP(RANK(T24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  score, 2, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T24" s="1"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="1" t="s">
+      <c r="D24" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$C$7, $B24+1, FALSE)),"",VLOOKUP(RANK(E24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$C$7, $B24+1, FALSE))</f>
+        <v>50</v>
+      </c>
+      <c r="E24" s="1">
+        <v>100</v>
+      </c>
+      <c r="G24" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$C$7, $B24+1, FALSE)),"",VLOOKUP(RANK(H24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$C$7, $B24+1, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$C$7, $B24+1, FALSE)),"",VLOOKUP(RANK(K24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$C$7, $B24+1, FALSE))</f>
+        <v>-15</v>
+      </c>
+      <c r="K24" s="1">
+        <v>40</v>
+      </c>
+      <c r="M24" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$C$7, $B24+1, FALSE)),"",VLOOKUP(RANK(N24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$C$7, $B24+1, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="N24" s="1">
+        <v>60</v>
+      </c>
+      <c r="P24" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$C$7, $B24+1, FALSE)),"",VLOOKUP(RANK(Q24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$C$7, $B24+1, FALSE))</f>
+        <v>20</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>80</v>
+      </c>
+      <c r="S24" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$C$7, $B24+1, FALSE)),"",VLOOKUP(RANK(T24, ($T24,$Q24,$N24,$K24,$H24,$E24), 0),  $A$2:$C$7, $B24+1, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="T24" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>16</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE)),"",VLOOKUP(RANK(E25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="G25" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE)),"",VLOOKUP(RANK(H25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="J25" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE)),"",VLOOKUP(RANK(K25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="M25" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE)),"",VLOOKUP(RANK(N25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N25" s="1"/>
+      <c r="P25" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE)),"",VLOOKUP(RANK(Q25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q25" s="1"/>
+      <c r="S25" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE)),"",VLOOKUP(RANK(T25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T25" s="1"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>17</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$C$7, $B26+1, FALSE)),"",VLOOKUP(RANK(E26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$C$7, $B26+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="G26" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$C$7, $B26+1, FALSE)),"",VLOOKUP(RANK(H26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$C$7, $B26+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="J26" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$C$7, $B26+1, FALSE)),"",VLOOKUP(RANK(K26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$C$7, $B26+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="M26" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$C$7, $B26+1, FALSE)),"",VLOOKUP(RANK(N26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$C$7, $B26+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N26" s="1"/>
+      <c r="P26" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$C$7, $B26+1, FALSE)),"",VLOOKUP(RANK(Q26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$C$7, $B26+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q26" s="1"/>
+      <c r="S26" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$C$7, $B26+1, FALSE)),"",VLOOKUP(RANK(T26, ($T26,$Q26,$N26,$K26,$H26,$E26), 0),  $A$2:$C$7, $B26+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T26" s="1"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>18</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE)),"",VLOOKUP(RANK(E27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="G27" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE)),"",VLOOKUP(RANK(H27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="J27" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE)),"",VLOOKUP(RANK(K27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K27" s="1"/>
+      <c r="M27" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE)),"",VLOOKUP(RANK(N27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N27" s="1"/>
+      <c r="P27" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE)),"",VLOOKUP(RANK(Q27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q27" s="1"/>
+      <c r="S27" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE)),"",VLOOKUP(RANK(T27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T27" s="1"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>19</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE)),"",VLOOKUP(RANK(E28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="G28" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE)),"",VLOOKUP(RANK(H28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="J28" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE)),"",VLOOKUP(RANK(K28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="M28" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE)),"",VLOOKUP(RANK(N28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N28" s="1"/>
+      <c r="P28" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE)),"",VLOOKUP(RANK(Q28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q28" s="1"/>
+      <c r="S28" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE)),"",VLOOKUP(RANK(T28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T28" s="1"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>20</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE)),"",VLOOKUP(RANK(E29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="G29" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE)),"",VLOOKUP(RANK(H29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="J29" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE)),"",VLOOKUP(RANK(K29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="M29" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE)),"",VLOOKUP(RANK(N29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N29" s="1"/>
+      <c r="P29" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE)),"",VLOOKUP(RANK(Q29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q29" s="1"/>
+      <c r="S29" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE)),"",VLOOKUP(RANK(T29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T29" s="1"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>21</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE)),"",VLOOKUP(RANK(E30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="G30" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE)),"",VLOOKUP(RANK(H30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="J30" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE)),"",VLOOKUP(RANK(K30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="M30" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE)),"",VLOOKUP(RANK(N30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N30" s="1"/>
+      <c r="P30" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE)),"",VLOOKUP(RANK(Q30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q30" s="1"/>
+      <c r="S30" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE)),"",VLOOKUP(RANK(T30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T30" s="1"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>22</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE)),"",VLOOKUP(RANK(E31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="G31" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE)),"",VLOOKUP(RANK(H31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="J31" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE)),"",VLOOKUP(RANK(K31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K31" s="1"/>
+      <c r="M31" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE)),"",VLOOKUP(RANK(N31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N31" s="1"/>
+      <c r="P31" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE)),"",VLOOKUP(RANK(Q31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q31" s="1"/>
+      <c r="S31" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE)),"",VLOOKUP(RANK(T31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T31" s="1"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>23</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE)),"",VLOOKUP(RANK(E32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="G32" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE)),"",VLOOKUP(RANK(H32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H32" s="1"/>
+      <c r="J32" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE)),"",VLOOKUP(RANK(K32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K32" s="1"/>
+      <c r="M32" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE)),"",VLOOKUP(RANK(N32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N32" s="1"/>
+      <c r="P32" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE)),"",VLOOKUP(RANK(Q32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q32" s="1"/>
+      <c r="S32" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE)),"",VLOOKUP(RANK(T32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T32" s="1"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>24</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE)),"",VLOOKUP(RANK(E33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="G33" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE)),"",VLOOKUP(RANK(H33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="J33" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE)),"",VLOOKUP(RANK(K33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K33" s="1"/>
+      <c r="M33" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE)),"",VLOOKUP(RANK(N33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N33" s="1"/>
+      <c r="P33" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE)),"",VLOOKUP(RANK(Q33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q33" s="1"/>
+      <c r="S33" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE)),"",VLOOKUP(RANK(T33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T33" s="1"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>25</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE)),"",VLOOKUP(RANK(E34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="G34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE)),"",VLOOKUP(RANK(H34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="J34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE)),"",VLOOKUP(RANK(K34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K34" s="1"/>
+      <c r="M34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE)),"",VLOOKUP(RANK(N34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N34" s="1"/>
+      <c r="P34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE)),"",VLOOKUP(RANK(Q34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q34" s="1"/>
+      <c r="S34" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE)),"",VLOOKUP(RANK(T34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T34" s="1"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>26</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE)),"",VLOOKUP(RANK(E35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="G35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE)),"",VLOOKUP(RANK(H35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="J35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE)),"",VLOOKUP(RANK(K35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K35" s="1"/>
+      <c r="M35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE)),"",VLOOKUP(RANK(N35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N35" s="1"/>
+      <c r="P35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE)),"",VLOOKUP(RANK(Q35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q35" s="1"/>
+      <c r="S35" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE)),"",VLOOKUP(RANK(T35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T35" s="1"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>27</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE)),"",VLOOKUP(RANK(E36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="G36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE)),"",VLOOKUP(RANK(H36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="J36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE)),"",VLOOKUP(RANK(K36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K36" s="1"/>
+      <c r="M36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE)),"",VLOOKUP(RANK(N36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N36" s="1"/>
+      <c r="P36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE)),"",VLOOKUP(RANK(Q36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q36" s="1"/>
+      <c r="S36" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE)),"",VLOOKUP(RANK(T36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T36" s="1"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>28</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE)),"",VLOOKUP(RANK(E37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="G37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE)),"",VLOOKUP(RANK(H37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="J37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE)),"",VLOOKUP(RANK(K37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K37" s="1"/>
+      <c r="M37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE)),"",VLOOKUP(RANK(N37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N37" s="1"/>
+      <c r="P37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE)),"",VLOOKUP(RANK(Q37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q37" s="1"/>
+      <c r="S37" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE)),"",VLOOKUP(RANK(T37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T37" s="1"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>29</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE)),"",VLOOKUP(RANK(E38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="G38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE)),"",VLOOKUP(RANK(H38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="J38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE)),"",VLOOKUP(RANK(K38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K38" s="1"/>
+      <c r="M38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE)),"",VLOOKUP(RANK(N38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N38" s="1"/>
+      <c r="P38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE)),"",VLOOKUP(RANK(Q38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q38" s="1"/>
+      <c r="S38" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE)),"",VLOOKUP(RANK(T38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T38" s="1"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>30</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(E39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="G39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(H39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H39" s="1"/>
+      <c r="J39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(K39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K39" s="1"/>
+      <c r="M39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(N39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N39" s="1"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="1"/>
+      <c r="S39" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(T39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T39" s="1"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A40" s="5"/>
+      <c r="B40" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="8" t="s">
+      <c r="C40" s="9"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="8" t="s">
+      <c r="G40" s="1"/>
+      <c r="H40" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="8" t="s">
+      <c r="J40" s="1"/>
+      <c r="K40" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M25" s="1"/>
-      <c r="N25" s="8" t="s">
+      <c r="M40" s="1"/>
+      <c r="N40" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="8" t="s">
+      <c r="P40" s="1"/>
+      <c r="Q40" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="S25" s="1"/>
-      <c r="T25" s="8" t="s">
+      <c r="S40" s="1"/>
+      <c r="T40" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="10" t="str">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="10" t="str">
         <f>D9</f>
         <v>Anantha</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="10" t="str">
+      <c r="G41" s="1"/>
+      <c r="H41" s="10" t="str">
         <f>G9</f>
         <v>Jayanth</v>
       </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="10" t="str">
+      <c r="J41" s="1"/>
+      <c r="K41" s="10" t="str">
         <f>J9</f>
         <v>Justin</v>
       </c>
-      <c r="M26" s="1"/>
-      <c r="N26" s="10" t="str">
+      <c r="M41" s="1"/>
+      <c r="N41" s="10" t="str">
         <f>M9</f>
         <v>Rapaka</v>
       </c>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="10" t="str">
+      <c r="P41" s="1"/>
+      <c r="Q41" s="10" t="str">
         <f>P9</f>
         <v>Sushma</v>
       </c>
-      <c r="S26" s="1"/>
-      <c r="T26" s="10" t="str">
+      <c r="S41" s="1"/>
+      <c r="T41" s="10" t="str">
         <f>S9</f>
         <v>Sampath M</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="6" t="s">
+    <row r="42" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E42" s="11">
         <f>SUM(D10:D24)</f>
-        <v>37.5</v>
-      </c>
-      <c r="G27" s="6" t="s">
+        <v>67.5</v>
+      </c>
+      <c r="G42" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="11">
+      <c r="H42" s="11">
         <f>SUM(G10:G24)</f>
-        <v>-32.5</v>
-      </c>
-      <c r="J27" s="6" t="s">
+        <v>-107.5</v>
+      </c>
+      <c r="J42" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K27" s="11">
+      <c r="K42" s="11">
         <f>SUM(J10:J24)</f>
-        <v>-50</v>
-      </c>
-      <c r="M27" s="6" t="s">
+        <v>-40</v>
+      </c>
+      <c r="M42" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N27" s="11">
+      <c r="N42" s="11">
         <f>SUM(M10:M24)</f>
-        <v>20</v>
-      </c>
-      <c r="P27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P42" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q27" s="11">
+      <c r="Q42" s="11">
         <f>SUM(P10:P24)</f>
-        <v>60</v>
-      </c>
-      <c r="S27" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="S42" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="T27" s="11">
+      <c r="T42" s="11">
         <f>SUM(S10:S24)</f>
-        <v>-35</v>
-      </c>
-      <c r="U27" s="1">
-        <f>SUM(E27,H27,K27,N27,Q27,T27)</f>
+        <v>-65</v>
+      </c>
+      <c r="U42" s="1">
+        <f>SUM(E42,H42,K42,N42,Q42,T42)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2204,7 +2922,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E27">
+  <conditionalFormatting sqref="E42">
     <cfRule type="cellIs" dxfId="32" priority="76" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2215,7 +2933,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
+  <conditionalFormatting sqref="H42">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2226,7 +2944,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27">
+  <conditionalFormatting sqref="K42">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2237,7 +2955,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N27">
+  <conditionalFormatting sqref="N42">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2248,7 +2966,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q27">
+  <conditionalFormatting sqref="Q42">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2259,7 +2977,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27">
+  <conditionalFormatting sqref="T42">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2279,7 +2997,7 @@
   <dimension ref="F17:J60"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="D25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Contest 16 RCB vs RR
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230DC6FC-403F-AF46-AB54-9AE0211F3CE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B842452D-9776-C24F-B5F3-6C653E261F3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="4400" windowWidth="22700" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="1440" yWindow="4400" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -527,7 +527,157 @@
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="48">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1170,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
@@ -2061,35 +2211,35 @@
         <v>14</v>
       </c>
       <c r="B23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>54</v>
       </c>
       <c r="D23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE)),"",VLOOKUP(RANK(E23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE))</f>
-        <v>-25</v>
+        <v>-20</v>
       </c>
       <c r="E23" s="1">
         <v>20</v>
       </c>
       <c r="G23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE)),"",VLOOKUP(RANK(H23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE))</f>
-        <v>-20</v>
+        <v>-15</v>
       </c>
       <c r="H23" s="1">
         <v>40</v>
       </c>
       <c r="J23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE)),"",VLOOKUP(RANK(K23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE))</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K23" s="1">
         <v>100</v>
       </c>
       <c r="M23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE)),"",VLOOKUP(RANK(N23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE))</f>
-        <v>0</v>
+        <v>-25</v>
       </c>
       <c r="N23" s="1">
         <v>0</v>
@@ -2103,7 +2253,7 @@
       </c>
       <c r="S23" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE)),"",VLOOKUP(RANK(T23, ($T23,$Q23,$N23,$K23,$H23,$E23), 0),  $A$2:$C$7, $B23+1, FALSE))</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="T23" s="1">
         <v>80</v>
@@ -2172,36 +2322,48 @@
       <c r="C25" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="3" t="str">
+      <c r="D25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE)),"",VLOOKUP(RANK(E25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="G25" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE)),"",VLOOKUP(RANK(H25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H25" s="1"/>
-      <c r="J25" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H25" s="1">
+        <v>100</v>
+      </c>
+      <c r="J25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE)),"",VLOOKUP(RANK(K25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K25" s="1"/>
-      <c r="M25" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K25" s="1">
+        <v>20</v>
+      </c>
+      <c r="M25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE)),"",VLOOKUP(RANK(N25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N25" s="1"/>
-      <c r="P25" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N25" s="1">
+        <v>40</v>
+      </c>
+      <c r="P25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE)),"",VLOOKUP(RANK(Q25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q25" s="1"/>
-      <c r="S25" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>60</v>
+      </c>
+      <c r="S25" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE)),"",VLOOKUP(RANK(T25, ($T25,$Q25,$N25,$K25,$H25,$E25), 0),  $A$2:$C$7, $B25+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T25" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="T25" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -2848,43 +3010,43 @@
         <v>12</v>
       </c>
       <c r="E42" s="11">
-        <f>SUM(D10:D24)</f>
-        <v>67.5</v>
+        <f>SUM(D10:D39)</f>
+        <v>47.5</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H42" s="11">
-        <f>SUM(G10:G24)</f>
-        <v>-107.5</v>
+        <f>SUM(G10:G39)</f>
+        <v>-52.5</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K42" s="11">
-        <f>SUM(J10:J24)</f>
-        <v>-40</v>
+        <f>SUM(J10:J39)</f>
+        <v>-50</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N42" s="11">
-        <f>SUM(M10:M24)</f>
-        <v>35</v>
+        <f>SUM(M10:M39)</f>
+        <v>-5</v>
       </c>
       <c r="P42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q42" s="11">
-        <f>SUM(P10:P24)</f>
-        <v>110</v>
+        <f>SUM(P10:P39)</f>
+        <v>100</v>
       </c>
       <c r="S42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T42" s="11">
-        <f>SUM(S10:S24)</f>
-        <v>-65</v>
+        <f>SUM(S10:S39)</f>
+        <v>-40</v>
       </c>
       <c r="U42" s="1">
         <f>SUM(E42,H42,K42,N42,Q42,T42)</f>
@@ -2923,13 +3085,13 @@
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
   <conditionalFormatting sqref="E42">
-    <cfRule type="cellIs" dxfId="32" priority="76" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="91" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="92" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="78" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="93" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
contest 18 RR vs KKR
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349605BE-DF0F-9649-845F-6F86C2BB977D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7FA719-6431-C144-BFA3-61D6220B5187}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="3320" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -2428,36 +2428,48 @@
       <c r="C27" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="3" t="str">
+      <c r="D27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE)),"",VLOOKUP(RANK(E27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="G27" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E27" s="1">
+        <v>40</v>
+      </c>
+      <c r="G27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE)),"",VLOOKUP(RANK(H27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H27" s="1"/>
-      <c r="J27" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H27" s="1">
+        <v>60</v>
+      </c>
+      <c r="J27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE)),"",VLOOKUP(RANK(K27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K27" s="1"/>
-      <c r="M27" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K27" s="1">
+        <v>20</v>
+      </c>
+      <c r="M27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE)),"",VLOOKUP(RANK(N27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N27" s="1"/>
-      <c r="P27" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="N27" s="1">
+        <v>100</v>
+      </c>
+      <c r="P27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE)),"",VLOOKUP(RANK(Q27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q27" s="1"/>
-      <c r="S27" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>80</v>
+      </c>
+      <c r="S27" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE)),"",VLOOKUP(RANK(T27, ($T27,$Q27,$N27,$K27,$H27,$E27), 0),  $A$2:$C$7, $B27+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T27" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T27" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -3023,42 +3035,42 @@
       </c>
       <c r="E42" s="11">
         <f>SUM(D10:D39)</f>
-        <v>37.5</v>
+        <v>22.5</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H42" s="11">
         <f>SUM(G10:G39)</f>
-        <v>-67.5</v>
+        <v>-77.5</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K42" s="11">
         <f>SUM(J10:J39)</f>
-        <v>-70</v>
+        <v>-90</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N42" s="11">
         <f>SUM(M10:M39)</f>
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="P42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q42" s="11">
         <f>SUM(P10:P39)</f>
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="S42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T42" s="11">
         <f>SUM(S10:S39)</f>
-        <v>-65</v>
+        <v>-90</v>
       </c>
       <c r="U42" s="1">
         <f>SUM(E42,H42,K42,N42,Q42,T42)</f>

</xml_diff>

<commit_message>
Contest 19 and 20
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7FA719-6431-C144-BFA3-61D6220B5187}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCA4A1A-5136-7D41-9A5D-30B13C3E09F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="3320" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -2481,36 +2481,48 @@
       <c r="C28" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="3" t="str">
+      <c r="D28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE)),"",VLOOKUP(RANK(E28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="G28" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="E28" s="1">
+        <v>100</v>
+      </c>
+      <c r="G28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE)),"",VLOOKUP(RANK(H28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H28" s="1"/>
-      <c r="J28" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1">
+        <v>80</v>
+      </c>
+      <c r="J28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE)),"",VLOOKUP(RANK(K28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K28" s="1"/>
-      <c r="M28" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K28" s="1">
+        <v>60</v>
+      </c>
+      <c r="M28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE)),"",VLOOKUP(RANK(N28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N28" s="1"/>
-      <c r="P28" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N28" s="1">
+        <v>40</v>
+      </c>
+      <c r="P28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE)),"",VLOOKUP(RANK(Q28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q28" s="1"/>
-      <c r="S28" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>0</v>
+      </c>
+      <c r="S28" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE)),"",VLOOKUP(RANK(T28, ($T28,$Q28,$N28,$K28,$H28,$E28), 0),  $A$2:$C$7, $B28+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T28" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="T28" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -2522,36 +2534,48 @@
       <c r="C29" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="3" t="str">
+      <c r="D29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE)),"",VLOOKUP(RANK(E29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="G29" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E29" s="1">
+        <v>20</v>
+      </c>
+      <c r="G29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE)),"",VLOOKUP(RANK(H29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H29" s="1"/>
-      <c r="J29" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H29" s="1">
+        <v>40</v>
+      </c>
+      <c r="J29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE)),"",VLOOKUP(RANK(K29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K29" s="1"/>
-      <c r="M29" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K29" s="1">
+        <v>100</v>
+      </c>
+      <c r="M29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE)),"",VLOOKUP(RANK(N29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N29" s="1"/>
-      <c r="P29" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N29" s="1">
+        <v>60</v>
+      </c>
+      <c r="P29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE)),"",VLOOKUP(RANK(Q29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q29" s="1"/>
-      <c r="S29" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>0</v>
+      </c>
+      <c r="S29" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE)),"",VLOOKUP(RANK(T29, ($T29,$Q29,$N29,$K29,$H29,$E29), 0),  $A$2:$C$7, $B29+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T29" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="T29" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -3035,35 +3059,35 @@
       </c>
       <c r="E42" s="11">
         <f>SUM(D10:D39)</f>
-        <v>22.5</v>
+        <v>52.5</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H42" s="11">
         <f>SUM(G10:G39)</f>
-        <v>-77.5</v>
+        <v>-72.5</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K42" s="11">
         <f>SUM(J10:J39)</f>
-        <v>-90</v>
+        <v>-50</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N42" s="11">
         <f>SUM(M10:M39)</f>
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="P42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q42" s="11">
         <f>SUM(P10:P39)</f>
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="S42" s="6" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
contest 21 PBKS vs KKR
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCA4A1A-5136-7D41-9A5D-30B13C3E09F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6D5C71-8CA8-4349-94CD-B3CD98CC8782}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="3320" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -2587,36 +2587,48 @@
       <c r="C30" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="3" t="str">
+      <c r="D30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE)),"",VLOOKUP(RANK(E30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="G30" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE)),"",VLOOKUP(RANK(H30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H30" s="1"/>
-      <c r="J30" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H30" s="1">
+        <v>60</v>
+      </c>
+      <c r="J30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE)),"",VLOOKUP(RANK(K30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K30" s="1"/>
-      <c r="M30" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="K30" s="1">
+        <v>80</v>
+      </c>
+      <c r="M30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE)),"",VLOOKUP(RANK(N30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N30" s="1"/>
-      <c r="P30" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="N30" s="1">
+        <v>40</v>
+      </c>
+      <c r="P30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE)),"",VLOOKUP(RANK(Q30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q30" s="1"/>
-      <c r="S30" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>20</v>
+      </c>
+      <c r="S30" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE)),"",VLOOKUP(RANK(T30, ($T30,$Q30,$N30,$K30,$H30,$E30), 0),  $A$2:$C$7, $B30+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T30" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="T30" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -3059,42 +3071,42 @@
       </c>
       <c r="E42" s="11">
         <f>SUM(D10:D39)</f>
-        <v>52.5</v>
+        <v>27.5</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H42" s="11">
         <f>SUM(G10:G39)</f>
-        <v>-72.5</v>
+        <v>-82.5</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K42" s="11">
         <f>SUM(J10:J39)</f>
-        <v>-50</v>
+        <v>-30</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N42" s="11">
         <f>SUM(M10:M39)</f>
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="P42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q42" s="11">
         <f>SUM(P10:P39)</f>
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="S42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T42" s="11">
         <f>SUM(S10:S39)</f>
-        <v>-90</v>
+        <v>-40</v>
       </c>
       <c r="U42" s="1">
         <f>SUM(E42,H42,K42,N42,Q42,T42)</f>

</xml_diff>

<commit_message>
Contest 22 DC vs RCB.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6D5C71-8CA8-4349-94CD-B3CD98CC8782}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD3AEE9-D1C8-574A-9134-2CF203777BC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="3320" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="860" yWindow="3960" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -507,6 +507,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -519,7 +520,6 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -527,307 +527,7 @@
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1353,15 +1053,15 @@
       <c r="C2" s="7">
         <v>40</v>
       </c>
-      <c r="I2" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
+      <c r="I2" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
@@ -1373,13 +1073,13 @@
       <c r="C3" s="7">
         <v>15</v>
       </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
@@ -1391,13 +1091,13 @@
       <c r="C4" s="7">
         <v>-10</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
@@ -1409,13 +1109,13 @@
       <c r="C5" s="7">
         <v>-20</v>
       </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
@@ -1427,13 +1127,13 @@
       <c r="C6" s="7">
         <v>-25</v>
       </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
@@ -1447,30 +1147,30 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="G8" s="21" t="s">
+      <c r="E8" s="22"/>
+      <c r="G8" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="J8" s="21" t="s">
+      <c r="H8" s="22"/>
+      <c r="J8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="M8" s="21" t="s">
+      <c r="K8" s="22"/>
+      <c r="M8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="21"/>
-      <c r="P8" s="21" t="s">
+      <c r="N8" s="22"/>
+      <c r="P8" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="Q8" s="21"/>
-      <c r="S8" s="21" t="s">
+      <c r="Q8" s="22"/>
+      <c r="S8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="T8" s="21"/>
+      <c r="T8" s="22"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
@@ -2319,7 +2019,7 @@
       <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="20" t="s">
         <v>57</v>
       </c>
       <c r="D25" s="3">
@@ -2372,7 +2072,7 @@
       <c r="B26" s="1">
         <v>1</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="20" t="s">
         <v>58</v>
       </c>
       <c r="D26" s="3">
@@ -2425,7 +2125,7 @@
       <c r="B27" s="1">
         <v>1</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="20" t="s">
         <v>59</v>
       </c>
       <c r="D27" s="3">
@@ -2478,7 +2178,7 @@
       <c r="B28" s="1">
         <v>1</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="20" t="s">
         <v>60</v>
       </c>
       <c r="D28" s="3">
@@ -2531,7 +2231,7 @@
       <c r="B29" s="1">
         <v>1</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="20" t="s">
         <v>61</v>
       </c>
       <c r="D29" s="3">
@@ -2584,7 +2284,7 @@
       <c r="B30" s="1">
         <v>1</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="20" t="s">
         <v>62</v>
       </c>
       <c r="D30" s="3">
@@ -2637,39 +2337,51 @@
       <c r="B31" s="1">
         <v>1</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="3" t="str">
+      <c r="D31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE)),"",VLOOKUP(RANK(E31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="G31" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E31" s="1">
+        <v>40</v>
+      </c>
+      <c r="G31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE)),"",VLOOKUP(RANK(H31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H31" s="1"/>
-      <c r="J31" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE)),"",VLOOKUP(RANK(K31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K31" s="1"/>
-      <c r="M31" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K31" s="1">
+        <v>60</v>
+      </c>
+      <c r="M31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE)),"",VLOOKUP(RANK(N31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N31" s="1"/>
-      <c r="P31" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N31" s="1">
+        <v>80</v>
+      </c>
+      <c r="P31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE)),"",VLOOKUP(RANK(Q31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q31" s="1"/>
-      <c r="S31" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>20</v>
+      </c>
+      <c r="S31" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE)),"",VLOOKUP(RANK(T31, ($T31,$Q31,$N31,$K31,$H31,$E31), 0),  $A$2:$C$7, $B31+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T31" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="T31" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -2678,7 +2390,7 @@
       <c r="B32" s="1">
         <v>1</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="20" t="s">
         <v>64</v>
       </c>
       <c r="D32" s="3" t="str">
@@ -2719,7 +2431,7 @@
       <c r="B33" s="1">
         <v>1</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="20" t="s">
         <v>65</v>
       </c>
       <c r="D33" s="3" t="str">
@@ -2760,7 +2472,7 @@
       <c r="B34" s="1">
         <v>1</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="20" t="s">
         <v>66</v>
       </c>
       <c r="D34" s="3" t="str">
@@ -2801,7 +2513,7 @@
       <c r="B35" s="1">
         <v>1</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="20" t="s">
         <v>67</v>
       </c>
       <c r="D35" s="3" t="str">
@@ -2842,7 +2554,7 @@
       <c r="B36" s="1">
         <v>1</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="20" t="s">
         <v>68</v>
       </c>
       <c r="D36" s="3" t="str">
@@ -2883,7 +2595,7 @@
       <c r="B37" s="1">
         <v>1</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="20" t="s">
         <v>69</v>
       </c>
       <c r="D37" s="3" t="str">
@@ -2924,7 +2636,7 @@
       <c r="B38" s="1">
         <v>1</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="20" t="s">
         <v>70</v>
       </c>
       <c r="D38" s="3" t="str">
@@ -2965,7 +2677,7 @@
       <c r="B39" s="1">
         <v>1</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="20" t="s">
         <v>71</v>
       </c>
       <c r="D39" s="3" t="str">
@@ -3071,42 +2783,42 @@
       </c>
       <c r="E42" s="11">
         <f>SUM(D10:D39)</f>
-        <v>27.5</v>
+        <v>12.5</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H42" s="11">
         <f>SUM(G10:G39)</f>
-        <v>-82.5</v>
+        <v>-107.5</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K42" s="11">
         <f>SUM(J10:J39)</f>
-        <v>-30</v>
+        <v>-40</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N42" s="11">
         <f>SUM(M10:M39)</f>
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="P42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q42" s="11">
         <f>SUM(P10:P39)</f>
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="S42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T42" s="11">
         <f>SUM(S10:S39)</f>
-        <v>-40</v>
+        <v>10</v>
       </c>
       <c r="U42" s="1">
         <f>SUM(E42,H42,K42,N42,Q42,T42)</f>
@@ -3145,13 +2857,13 @@
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
   <conditionalFormatting sqref="E42">
-    <cfRule type="cellIs" dxfId="47" priority="91" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="91" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="92" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="93" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3248,7 +2960,7 @@
       </c>
     </row>
     <row r="19" spans="6:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I19" s="22" t="s">
+      <c r="I19" s="23" t="s">
         <v>23</v>
       </c>
       <c r="J19" s="13" t="s">
@@ -3256,7 +2968,7 @@
       </c>
     </row>
     <row r="20" spans="6:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I20" s="23"/>
+      <c r="I20" s="24"/>
       <c r="J20" s="13" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Contest 23 CSK vs SRH
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD3AEE9-D1C8-574A-9134-2CF203777BC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A995913-9D9F-F44E-8E01-398EA7AF2A63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="3960" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -2393,36 +2393,48 @@
       <c r="C32" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="3" t="str">
+      <c r="D32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE)),"",VLOOKUP(RANK(E32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E32" s="1"/>
-      <c r="G32" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE)),"",VLOOKUP(RANK(H32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H32" s="1"/>
-      <c r="J32" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H32" s="1">
+        <v>20</v>
+      </c>
+      <c r="J32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE)),"",VLOOKUP(RANK(K32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K32" s="1"/>
-      <c r="M32" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="K32" s="1">
+        <v>40</v>
+      </c>
+      <c r="M32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE)),"",VLOOKUP(RANK(N32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N32" s="1"/>
-      <c r="P32" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N32" s="1">
+        <v>80</v>
+      </c>
+      <c r="P32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE)),"",VLOOKUP(RANK(Q32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q32" s="1"/>
-      <c r="S32" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>100</v>
+      </c>
+      <c r="S32" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE)),"",VLOOKUP(RANK(T32, ($T32,$Q32,$N32,$K32,$H32,$E32), 0),  $A$2:$C$7, $B32+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T32" s="1"/>
+        <v>-10</v>
+      </c>
+      <c r="T32" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -2783,42 +2795,42 @@
       </c>
       <c r="E42" s="11">
         <f>SUM(D10:D39)</f>
-        <v>12.5</v>
+        <v>-12.5</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H42" s="11">
         <f>SUM(G10:G39)</f>
-        <v>-107.5</v>
+        <v>-127.5</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K42" s="11">
         <f>SUM(J10:J39)</f>
-        <v>-40</v>
+        <v>-55</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N42" s="11">
         <f>SUM(M10:M39)</f>
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="P42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q42" s="11">
         <f>SUM(P10:P39)</f>
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="S42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T42" s="11">
         <f>SUM(S10:S39)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U42" s="1">
         <f>SUM(E42,H42,K42,N42,Q42,T42)</f>

</xml_diff>

<commit_message>
Results: Contest 26 PBKS vs RCB
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A995913-9D9F-F44E-8E01-398EA7AF2A63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C019C2-19FE-064C-B3A0-C7FC3D1F4772}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="3960" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -2446,36 +2446,46 @@
       <c r="C33" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE)),"",VLOOKUP(RANK(E33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="G33" s="3" t="str">
+      <c r="D33" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="E33" s="1">
+        <v>20</v>
+      </c>
+      <c r="G33" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE)),"",VLOOKUP(RANK(H33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H33" s="1"/>
-      <c r="J33" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="H33" s="1">
+        <v>40</v>
+      </c>
+      <c r="J33" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE)),"",VLOOKUP(RANK(K33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K33" s="1"/>
-      <c r="M33" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K33" s="1">
+        <v>100</v>
+      </c>
+      <c r="M33" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE)),"",VLOOKUP(RANK(N33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N33" s="1"/>
-      <c r="P33" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N33" s="1">
+        <v>80</v>
+      </c>
+      <c r="P33" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE)),"",VLOOKUP(RANK(Q33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q33" s="1"/>
-      <c r="S33" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE)),"",VLOOKUP(RANK(T33, ($T33,$Q33,$N33,$K33,$H33,$E33), 0),  $A$2:$C$7, $B33+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T33" s="1"/>
+        <v>-10</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>60</v>
+      </c>
+      <c r="S33" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="T33" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
@@ -2487,36 +2497,46 @@
       <c r="C34" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="3" t="str">
+      <c r="D34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE)),"",VLOOKUP(RANK(E34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="G34" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE)),"",VLOOKUP(RANK(H34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H34" s="1"/>
-      <c r="J34" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H34" s="1">
+        <v>60</v>
+      </c>
+      <c r="J34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE)),"",VLOOKUP(RANK(K34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K34" s="1"/>
-      <c r="M34" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K34" s="1">
+        <v>20</v>
+      </c>
+      <c r="M34" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE)),"",VLOOKUP(RANK(N34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N34" s="1"/>
-      <c r="P34" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Q34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE)),"",VLOOKUP(RANK(Q34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q34" s="1"/>
-      <c r="S34" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE)),"",VLOOKUP(RANK(T34, ($T34,$Q34,$N34,$K34,$H34,$E34), 0),  $A$2:$C$7, $B34+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T34" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="N34" s="1">
+        <v>40</v>
+      </c>
+      <c r="P34" s="3">
+        <v>35</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>100</v>
+      </c>
+      <c r="S34" s="3">
+        <v>35</v>
+      </c>
+      <c r="T34" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -2528,36 +2548,48 @@
       <c r="C35" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="3" t="str">
+      <c r="D35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE)),"",VLOOKUP(RANK(E35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E35" s="1"/>
-      <c r="G35" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE)),"",VLOOKUP(RANK(H35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H35" s="1"/>
-      <c r="J35" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H35" s="1">
+        <v>60</v>
+      </c>
+      <c r="J35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE)),"",VLOOKUP(RANK(K35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K35" s="1"/>
-      <c r="M35" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K35" s="1">
+        <v>100</v>
+      </c>
+      <c r="M35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE)),"",VLOOKUP(RANK(N35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N35" s="1"/>
-      <c r="P35" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N35" s="1">
+        <v>80</v>
+      </c>
+      <c r="P35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE)),"",VLOOKUP(RANK(Q35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q35" s="1"/>
-      <c r="S35" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>20</v>
+      </c>
+      <c r="S35" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE)),"",VLOOKUP(RANK(T35, ($T35,$Q35,$N35,$K35,$H35,$E35), 0),  $A$2:$C$7, $B35+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T35" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="T35" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -2795,42 +2827,42 @@
       </c>
       <c r="E42" s="11">
         <f>SUM(D10:D39)</f>
-        <v>-12.5</v>
+        <v>-85</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H42" s="11">
         <f>SUM(G10:G39)</f>
-        <v>-127.5</v>
+        <v>-162.5</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K42" s="11">
         <f>SUM(J10:J39)</f>
-        <v>-55</v>
+        <v>25</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N42" s="11">
         <f>SUM(M10:M39)</f>
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="P42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q42" s="11">
         <f>SUM(P10:P39)</f>
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="S42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T42" s="11">
         <f>SUM(S10:S39)</f>
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="U42" s="1">
         <f>SUM(E42,H42,K42,N42,Q42,T42)</f>

</xml_diff>

<commit_message>
contest 27 mi vs csk
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C019C2-19FE-064C-B3A0-C7FC3D1F4772}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE539292-2391-C941-88E8-CE8A8FC7762F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="3960" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="380" yWindow="3980" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2601,36 +2601,48 @@
       <c r="C36" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="3" t="str">
+      <c r="D36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE)),"",VLOOKUP(RANK(E36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="G36" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="E36" s="1">
+        <v>40</v>
+      </c>
+      <c r="G36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE)),"",VLOOKUP(RANK(H36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="J36" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="H36" s="1">
+        <v>80</v>
+      </c>
+      <c r="J36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE)),"",VLOOKUP(RANK(K36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K36" s="1"/>
-      <c r="M36" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K36" s="1">
+        <v>20</v>
+      </c>
+      <c r="M36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE)),"",VLOOKUP(RANK(N36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N36" s="1"/>
-      <c r="P36" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
+      <c r="P36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE)),"",VLOOKUP(RANK(Q36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q36" s="1"/>
-      <c r="S36" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>60</v>
+      </c>
+      <c r="S36" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE)),"",VLOOKUP(RANK(T36, ($T36,$Q36,$N36,$K36,$H36,$E36), 0),  $A$2:$C$7, $B36+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T36" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="T36" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -2827,42 +2839,42 @@
       </c>
       <c r="E42" s="11">
         <f>SUM(D10:D39)</f>
-        <v>-85</v>
+        <v>-100</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H42" s="11">
         <f>SUM(G10:G39)</f>
-        <v>-162.5</v>
+        <v>-142.5</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K42" s="11">
         <f>SUM(J10:J39)</f>
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N42" s="11">
         <f>SUM(M10:M39)</f>
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="P42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q42" s="11">
         <f>SUM(P10:P39)</f>
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="S42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T42" s="11">
         <f>SUM(S10:S39)</f>
-        <v>-2.5</v>
+        <v>47.5</v>
       </c>
       <c r="U42" s="1">
         <f>SUM(E42,H42,K42,N42,Q42,T42)</f>

</xml_diff>

<commit_message>
results contest 28 and 29
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE539292-2391-C941-88E8-CE8A8FC7762F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1E4676-1062-0044-8138-60EFAE713F6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="3980" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -2654,36 +2654,48 @@
       <c r="C37" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="3" t="str">
+      <c r="D37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE)),"",VLOOKUP(RANK(E37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="G37" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E37" s="1">
+        <v>20</v>
+      </c>
+      <c r="G37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE)),"",VLOOKUP(RANK(H37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H37" s="1"/>
-      <c r="J37" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H37" s="1">
+        <v>60</v>
+      </c>
+      <c r="J37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE)),"",VLOOKUP(RANK(K37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K37" s="1"/>
-      <c r="M37" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="K37" s="1">
+        <v>100</v>
+      </c>
+      <c r="M37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE)),"",VLOOKUP(RANK(N37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N37" s="1"/>
-      <c r="P37" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N37" s="1">
+        <v>80</v>
+      </c>
+      <c r="P37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE)),"",VLOOKUP(RANK(Q37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q37" s="1"/>
-      <c r="S37" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>0</v>
+      </c>
+      <c r="S37" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE)),"",VLOOKUP(RANK(T37, ($T37,$Q37,$N37,$K37,$H37,$E37), 0),  $A$2:$C$7, $B37+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T37" s="1"/>
+        <v>-15</v>
+      </c>
+      <c r="T37" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
@@ -2695,36 +2707,48 @@
       <c r="C38" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="3" t="str">
+      <c r="D38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE)),"",VLOOKUP(RANK(E38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E38" s="1"/>
-      <c r="G38" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E38" s="1">
+        <v>20</v>
+      </c>
+      <c r="G38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE)),"",VLOOKUP(RANK(H38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H38" s="1"/>
-      <c r="J38" s="3" t="str">
+        <v>50</v>
+      </c>
+      <c r="H38" s="1">
+        <v>100</v>
+      </c>
+      <c r="J38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE)),"",VLOOKUP(RANK(K38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K38" s="1"/>
-      <c r="M38" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K38" s="1">
+        <v>60</v>
+      </c>
+      <c r="M38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE)),"",VLOOKUP(RANK(N38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N38" s="1"/>
-      <c r="P38" s="3" t="str">
+        <v>20</v>
+      </c>
+      <c r="N38" s="1">
+        <v>80</v>
+      </c>
+      <c r="P38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE)),"",VLOOKUP(RANK(Q38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q38" s="1"/>
-      <c r="S38" s="3" t="str">
+        <v>-15</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>40</v>
+      </c>
+      <c r="S38" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE)),"",VLOOKUP(RANK(T38, ($T38,$Q38,$N38,$K38,$H38,$E38), 0),  $A$2:$C$7, $B38+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T38" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T38" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
@@ -2839,42 +2863,42 @@
       </c>
       <c r="E42" s="11">
         <f>SUM(D10:D39)</f>
-        <v>-100</v>
+        <v>-140</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H42" s="11">
         <f>SUM(G10:G39)</f>
-        <v>-142.5</v>
+        <v>-102.5</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K42" s="11">
         <f>SUM(J10:J39)</f>
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N42" s="11">
         <f>SUM(M10:M39)</f>
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="P42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q42" s="11">
         <f>SUM(P10:P39)</f>
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="S42" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T42" s="11">
         <f>SUM(S10:S39)</f>
-        <v>47.5</v>
+        <v>7.5</v>
       </c>
       <c r="U42" s="1">
         <f>SUM(E42,H42,K42,N42,Q42,T42)</f>

</xml_diff>

<commit_message>
results contest 30 csk vs mi.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1E4676-1062-0044-8138-60EFAE713F6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED990F55-B769-DA4E-879E-7573630ED84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="3980" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="1620" yWindow="3940" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="76">
   <si>
     <t>Points</t>
   </si>
@@ -248,6 +248,18 @@
   </si>
   <si>
     <t>KKR vs RCB</t>
+  </si>
+  <si>
+    <t>CSK vs MI</t>
+  </si>
+  <si>
+    <t>PBKS vs RR</t>
+  </si>
+  <si>
+    <t>DC vs SRH</t>
+  </si>
+  <si>
+    <t>MI vs KKR</t>
   </si>
 </sst>
 </file>
@@ -1018,11 +1030,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U45"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U42" sqref="U42"/>
+      <selection pane="bottomLeft" activeCell="U46" sqref="U46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2755,176 +2767,355 @@
         <v>30</v>
       </c>
       <c r="B39" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(E39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+        <v>15</v>
+      </c>
+      <c r="E39" s="1">
+        <v>80</v>
+      </c>
+      <c r="G39" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(H39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="H39" s="1">
+        <v>20</v>
+      </c>
+      <c r="J39" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(K39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="K39" s="1">
+        <v>60</v>
+      </c>
+      <c r="M39" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(N39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+        <v>40</v>
+      </c>
+      <c r="N39" s="1">
+        <v>100</v>
+      </c>
+      <c r="P39" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(Q39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>0</v>
+      </c>
+      <c r="S39" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(T39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="T39" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>31</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2</v>
+      </c>
+      <c r="C40" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(E39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(E39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+      <c r="D40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE)),"",VLOOKUP(RANK(E40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE))</f>
         <v/>
       </c>
-      <c r="E39" s="1"/>
-      <c r="G39" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(H39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+      <c r="E40" s="1"/>
+      <c r="G40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE)),"",VLOOKUP(RANK(H40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE))</f>
         <v/>
       </c>
-      <c r="H39" s="1"/>
-      <c r="J39" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(K39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+      <c r="H40" s="1"/>
+      <c r="J40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE)),"",VLOOKUP(RANK(K40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE))</f>
         <v/>
       </c>
-      <c r="K39" s="1"/>
-      <c r="M39" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(N39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+      <c r="K40" s="1"/>
+      <c r="M40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE)),"",VLOOKUP(RANK(N40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE))</f>
         <v/>
       </c>
-      <c r="N39" s="1"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="1"/>
-      <c r="S39" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE)),"",VLOOKUP(RANK(T39, ($T39,$Q39,$N39,$K39,$H39,$E39), 0),  $A$2:$C$7, $B39+1, FALSE))</f>
+      <c r="N40" s="1"/>
+      <c r="P40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE)),"",VLOOKUP(RANK(Q40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE))</f>
         <v/>
       </c>
-      <c r="T39" s="1"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A40" s="5"/>
-      <c r="B40" s="1" t="s">
+      <c r="Q40" s="1"/>
+      <c r="S40" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE)),"",VLOOKUP(RANK(T40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T40" s="1"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>32</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE)),"",VLOOKUP(RANK(E41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="G41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE)),"",VLOOKUP(RANK(H41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="J41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE)),"",VLOOKUP(RANK(K41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K41" s="1"/>
+      <c r="M41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE)),"",VLOOKUP(RANK(N41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N41" s="1"/>
+      <c r="P41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE)),"",VLOOKUP(RANK(Q41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q41" s="1"/>
+      <c r="S41" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE)),"",VLOOKUP(RANK(T41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T41" s="1"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>33</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE)),"",VLOOKUP(RANK(E42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="G42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE)),"",VLOOKUP(RANK(H42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H42" s="1"/>
+      <c r="J42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE)),"",VLOOKUP(RANK(K42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K42" s="1"/>
+      <c r="M42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE)),"",VLOOKUP(RANK(N42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N42" s="1"/>
+      <c r="P42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE)),"",VLOOKUP(RANK(Q42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q42" s="1"/>
+      <c r="S42" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE)),"",VLOOKUP(RANK(T42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T42" s="1"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>34</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE)),"",VLOOKUP(RANK(E43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="G43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE)),"",VLOOKUP(RANK(H43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H43" s="1"/>
+      <c r="J43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE)),"",VLOOKUP(RANK(K43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K43" s="1"/>
+      <c r="M43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE)),"",VLOOKUP(RANK(N43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N43" s="1"/>
+      <c r="P43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE)),"",VLOOKUP(RANK(Q43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q43" s="1"/>
+      <c r="S43" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE)),"",VLOOKUP(RANK(T43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T43" s="1"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A44" s="5"/>
+      <c r="B44" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="8" t="s">
+      <c r="C44" s="9"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="8" t="s">
+      <c r="G44" s="1"/>
+      <c r="H44" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J40" s="1"/>
-      <c r="K40" s="8" t="s">
+      <c r="J44" s="1"/>
+      <c r="K44" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M40" s="1"/>
-      <c r="N40" s="8" t="s">
+      <c r="M44" s="1"/>
+      <c r="N44" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="8" t="s">
+      <c r="P44" s="1"/>
+      <c r="Q44" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="S40" s="1"/>
-      <c r="T40" s="8" t="s">
+      <c r="S44" s="1"/>
+      <c r="T44" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="10" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="10" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J41" s="1"/>
-      <c r="K41" s="10" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M41" s="1"/>
-      <c r="N41" s="10" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="10" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S41" s="1"/>
-      <c r="T41" s="10" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42" s="11">
-        <f>SUM(D10:D39)</f>
-        <v>-140</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" s="11">
-        <f>SUM(G10:G39)</f>
-        <v>-102.5</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K42" s="11">
-        <f>SUM(J10:J39)</f>
-        <v>45</v>
-      </c>
-      <c r="M42" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N42" s="11">
-        <f>SUM(M10:M39)</f>
-        <v>105</v>
-      </c>
-      <c r="P42" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q42" s="11">
-        <f>SUM(P10:P39)</f>
-        <v>85</v>
-      </c>
-      <c r="S42" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="T42" s="11">
-        <f>SUM(S10:S39)</f>
-        <v>7.5</v>
-      </c>
-      <c r="U42" s="1">
-        <f>SUM(E42,H42,K42,N42,Q42,T42)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="10" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G45" s="1"/>
+      <c r="H45" s="10" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J45" s="1"/>
+      <c r="K45" s="10" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M45" s="1"/>
+      <c r="N45" s="10" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="10" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S45" s="1"/>
+      <c r="T45" s="10" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="11">
+        <f>SUM(D10:D43)</f>
+        <v>-125</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="11">
+        <f>SUM(G10:G43)</f>
+        <v>-127.5</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K46" s="11">
+        <f>SUM(J10:J43)</f>
+        <v>35</v>
+      </c>
+      <c r="M46" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N46" s="11">
+        <f>SUM(M10:M43)</f>
+        <v>145</v>
+      </c>
+      <c r="P46" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q46" s="11">
+        <f>SUM(P10:P43)</f>
+        <v>85</v>
+      </c>
+      <c r="S46" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T46" s="11">
+        <f>SUM(S10:S43)</f>
+        <v>-12.5</v>
+      </c>
+      <c r="U46" s="1">
+        <f>SUM(E46,H46,K46,N46,Q46,T46)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2936,7 +3127,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E42">
+  <conditionalFormatting sqref="E46">
     <cfRule type="cellIs" dxfId="17" priority="91" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2947,7 +3138,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H42">
+  <conditionalFormatting sqref="H46">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2958,7 +3149,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K42">
+  <conditionalFormatting sqref="K46">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2969,7 +3160,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N42">
+  <conditionalFormatting sqref="N46">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2980,7 +3171,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q42">
+  <conditionalFormatting sqref="Q46">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -2991,7 +3182,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T42">
+  <conditionalFormatting sqref="T46">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Contest 31 KKR vs RCB
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED990F55-B769-DA4E-879E-7573630ED84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DB894F-30B3-6F46-9977-A8CA9A755152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="3940" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="760" yWindow="4000" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2825,36 +2825,48 @@
       <c r="C40" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="D40" s="3" t="str">
+      <c r="D40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE)),"",VLOOKUP(RANK(E40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E40" s="1"/>
-      <c r="G40" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="E40" s="1">
+        <v>100</v>
+      </c>
+      <c r="G40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE)),"",VLOOKUP(RANK(H40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H40" s="1"/>
-      <c r="J40" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="H40" s="1">
+        <v>80</v>
+      </c>
+      <c r="J40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE)),"",VLOOKUP(RANK(K40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K40" s="1"/>
-      <c r="M40" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K40" s="1">
+        <v>40</v>
+      </c>
+      <c r="M40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE)),"",VLOOKUP(RANK(N40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N40" s="1"/>
-      <c r="P40" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N40" s="1">
+        <v>60</v>
+      </c>
+      <c r="P40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE)),"",VLOOKUP(RANK(Q40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q40" s="1"/>
-      <c r="S40" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>0</v>
+      </c>
+      <c r="S40" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE)),"",VLOOKUP(RANK(T40, ($T40,$Q40,$N40,$K40,$H40,$E40), 0),  $A$2:$C$7, $B40+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T40" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T40" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
@@ -3054,28 +3066,28 @@
       </c>
       <c r="E46" s="11">
         <f>SUM(D10:D43)</f>
-        <v>-125</v>
+        <v>-85</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H46" s="11">
         <f>SUM(G10:G43)</f>
-        <v>-127.5</v>
+        <v>-112.5</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K46" s="11">
         <f>SUM(J10:J43)</f>
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="M46" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N46" s="11">
         <f>SUM(M10:M43)</f>
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="P46" s="6" t="s">
         <v>12</v>
@@ -3089,7 +3101,7 @@
       </c>
       <c r="T46" s="11">
         <f>SUM(S10:S43)</f>
-        <v>-12.5</v>
+        <v>-37.5</v>
       </c>
       <c r="U46" s="1">
         <f>SUM(E46,H46,K46,N46,Q46,T46)</f>

</xml_diff>

<commit_message>
Contest 32 PBKS vs RR.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DB894F-30B3-6F46-9977-A8CA9A755152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867FB3DF-D46A-D248-B023-6671724F4E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="4000" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -2878,36 +2878,48 @@
       <c r="C41" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="D41" s="3" t="str">
+      <c r="D41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE)),"",VLOOKUP(RANK(E41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E41" s="1"/>
-      <c r="G41" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E41" s="1">
+        <v>60</v>
+      </c>
+      <c r="G41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE)),"",VLOOKUP(RANK(H41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H41" s="1"/>
-      <c r="J41" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="H41" s="1">
+        <v>80</v>
+      </c>
+      <c r="J41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE)),"",VLOOKUP(RANK(K41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K41" s="1"/>
-      <c r="M41" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K41" s="1">
+        <v>40</v>
+      </c>
+      <c r="M41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE)),"",VLOOKUP(RANK(N41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N41" s="1"/>
-      <c r="P41" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N41" s="1">
+        <v>20</v>
+      </c>
+      <c r="P41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE)),"",VLOOKUP(RANK(Q41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q41" s="1"/>
-      <c r="S41" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>0</v>
+      </c>
+      <c r="S41" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE)),"",VLOOKUP(RANK(T41, ($T41,$Q41,$N41,$K41,$H41,$E41), 0),  $A$2:$C$7, $B41+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T41" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="T41" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
@@ -3066,28 +3078,28 @@
       </c>
       <c r="E46" s="11">
         <f>SUM(D10:D43)</f>
-        <v>-85</v>
+        <v>-95</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H46" s="11">
         <f>SUM(G10:G43)</f>
-        <v>-112.5</v>
+        <v>-97.5</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K46" s="11">
         <f>SUM(J10:J43)</f>
-        <v>15</v>
+        <v>-5</v>
       </c>
       <c r="M46" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N46" s="11">
         <f>SUM(M10:M43)</f>
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="P46" s="6" t="s">
         <v>12</v>
@@ -3101,7 +3113,7 @@
       </c>
       <c r="T46" s="11">
         <f>SUM(S10:S43)</f>
-        <v>-37.5</v>
+        <v>2.5</v>
       </c>
       <c r="U46" s="1">
         <f>SUM(E46,H46,K46,N46,Q46,T46)</f>

</xml_diff>

<commit_message>
Contest 33 DC vs SRH.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867FB3DF-D46A-D248-B023-6671724F4E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BD9D4D-791D-AF4E-BD72-57E5C4863CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="4000" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -2931,36 +2931,48 @@
       <c r="C42" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="3" t="str">
+      <c r="D42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE)),"",VLOOKUP(RANK(E42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="G42" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="E42" s="1">
+        <v>100</v>
+      </c>
+      <c r="G42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE)),"",VLOOKUP(RANK(H42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H42" s="1"/>
-      <c r="J42" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="H42" s="1">
+        <v>80</v>
+      </c>
+      <c r="J42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE)),"",VLOOKUP(RANK(K42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K42" s="1"/>
-      <c r="M42" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K42" s="1">
+        <v>40</v>
+      </c>
+      <c r="M42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE)),"",VLOOKUP(RANK(N42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N42" s="1"/>
-      <c r="P42" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N42" s="1">
+        <v>20</v>
+      </c>
+      <c r="P42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE)),"",VLOOKUP(RANK(Q42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q42" s="1"/>
-      <c r="S42" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>0</v>
+      </c>
+      <c r="S42" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE)),"",VLOOKUP(RANK(T42, ($T42,$Q42,$N42,$K42,$H42,$E42), 0),  $A$2:$C$7, $B42+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T42" s="1"/>
+        <v>-10</v>
+      </c>
+      <c r="T42" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
@@ -3078,28 +3090,28 @@
       </c>
       <c r="E46" s="11">
         <f>SUM(D10:D43)</f>
-        <v>-95</v>
+        <v>-55</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H46" s="11">
         <f>SUM(G10:G43)</f>
-        <v>-97.5</v>
+        <v>-82.5</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K46" s="11">
         <f>SUM(J10:J43)</f>
-        <v>-5</v>
+        <v>-25</v>
       </c>
       <c r="M46" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N46" s="11">
         <f>SUM(M10:M43)</f>
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="P46" s="6" t="s">
         <v>12</v>
@@ -3113,7 +3125,7 @@
       </c>
       <c r="T46" s="11">
         <f>SUM(S10:S43)</f>
-        <v>2.5</v>
+        <v>-7.5</v>
       </c>
       <c r="U46" s="1">
         <f>SUM(E46,H46,K46,N46,Q46,T46)</f>

</xml_diff>

<commit_message>
Contest 34 MI vs KKR.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BD9D4D-791D-AF4E-BD72-57E5C4863CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659CEE97-21A9-9146-A8F5-65BDA40794F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="4000" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="87">
   <si>
     <t>Points</t>
   </si>
@@ -260,6 +260,39 @@
   </si>
   <si>
     <t>MI vs KKR</t>
+  </si>
+  <si>
+    <t>RCB vs CSK</t>
+  </si>
+  <si>
+    <t>DC vs RR</t>
+  </si>
+  <si>
+    <t>SRH vs PBKS</t>
+  </si>
+  <si>
+    <t>CSK vs KKR</t>
+  </si>
+  <si>
+    <t>RCB vs MI</t>
+  </si>
+  <si>
+    <t>SRH vs RR</t>
+  </si>
+  <si>
+    <t>KKR vs DC</t>
+  </si>
+  <si>
+    <t>MI vs PBKS</t>
+  </si>
+  <si>
+    <t>RR vs RCB</t>
+  </si>
+  <si>
+    <t>SRH vs CSK</t>
+  </si>
+  <si>
+    <t>KKR vs PBKS</t>
   </si>
 </sst>
 </file>
@@ -1030,11 +1063,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U49"/>
+  <dimension ref="A1:U60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U46" sqref="U46"/>
+      <pane ySplit="8" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U57" sqref="U57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2448,7 +2481,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>24</v>
       </c>
@@ -2499,7 +2532,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>25</v>
       </c>
@@ -2550,7 +2583,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>26</v>
       </c>
@@ -2603,7 +2636,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>27</v>
       </c>
@@ -2656,7 +2689,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>28</v>
       </c>
@@ -2709,7 +2742,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>29</v>
       </c>
@@ -2762,7 +2795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>30</v>
       </c>
@@ -2815,7 +2848,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>31</v>
       </c>
@@ -2868,7 +2901,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>32</v>
       </c>
@@ -2921,7 +2954,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>33</v>
       </c>
@@ -2974,7 +3007,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>34</v>
       </c>
@@ -2984,174 +3017,439 @@
       <c r="C43" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D43" s="3" t="str">
+      <c r="D43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE)),"",VLOOKUP(RANK(E43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E43" s="1"/>
-      <c r="G43" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E43" s="1">
+        <v>40</v>
+      </c>
+      <c r="G43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE)),"",VLOOKUP(RANK(H43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H43" s="1"/>
-      <c r="J43" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H43" s="1">
+        <v>20</v>
+      </c>
+      <c r="J43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE)),"",VLOOKUP(RANK(K43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K43" s="1"/>
-      <c r="M43" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K43" s="1">
+        <v>60</v>
+      </c>
+      <c r="M43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE)),"",VLOOKUP(RANK(N43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N43" s="1"/>
-      <c r="P43" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="N43" s="1">
+        <v>100</v>
+      </c>
+      <c r="P43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE)),"",VLOOKUP(RANK(Q43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q43" s="1"/>
-      <c r="S43" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>0</v>
+      </c>
+      <c r="S43" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE)),"",VLOOKUP(RANK(T43, ($T43,$Q43,$N43,$K43,$H43,$E43), 0),  $A$2:$C$7, $B43+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T43" s="1"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A44" s="5"/>
-      <c r="B44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T43" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>35</v>
+      </c>
+      <c r="B44" s="1">
+        <v>2</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="1"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="1"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="1"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="1"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="1"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="1"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>36</v>
+      </c>
+      <c r="B45" s="1">
+        <v>2</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="1"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="1"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="1"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="1"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="1"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="1"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>37</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="1"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="1"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="1"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="1"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="1"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="1"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>38</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="1"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="1"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="1"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="1"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="1"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="1"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>39</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="1"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="1"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="1"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="1"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="1"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="1"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>40</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="1"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="1"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="1"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="1"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="1"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="1"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>41</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="1"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="1"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="1"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="1"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="1"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="1"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>42</v>
+      </c>
+      <c r="B51" s="1">
+        <v>2</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="1"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="1"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="1"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="1"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="1"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="1"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>43</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="1"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="1"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="1"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="1"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="1"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="1"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>44</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="1"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="1"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="1"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="1"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="1"/>
+      <c r="S53" s="3"/>
+      <c r="T53" s="1"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
+        <v>45</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="1"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="1"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="1"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="1"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="1"/>
+      <c r="S54" s="3"/>
+      <c r="T54" s="1"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A55" s="5"/>
+      <c r="B55" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="8" t="s">
+      <c r="C55" s="9"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G44" s="1"/>
-      <c r="H44" s="8" t="s">
+      <c r="G55" s="1"/>
+      <c r="H55" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J44" s="1"/>
-      <c r="K44" s="8" t="s">
+      <c r="J55" s="1"/>
+      <c r="K55" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M44" s="1"/>
-      <c r="N44" s="8" t="s">
+      <c r="M55" s="1"/>
+      <c r="N55" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="8" t="s">
+      <c r="P55" s="1"/>
+      <c r="Q55" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="S44" s="1"/>
-      <c r="T44" s="8" t="s">
+      <c r="S55" s="1"/>
+      <c r="T55" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="10" t="str">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="10" t="str">
         <f>D9</f>
         <v>Anantha</v>
       </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="10" t="str">
+      <c r="G56" s="1"/>
+      <c r="H56" s="10" t="str">
         <f>G9</f>
         <v>Jayanth</v>
       </c>
-      <c r="J45" s="1"/>
-      <c r="K45" s="10" t="str">
+      <c r="J56" s="1"/>
+      <c r="K56" s="10" t="str">
         <f>J9</f>
         <v>Justin</v>
       </c>
-      <c r="M45" s="1"/>
-      <c r="N45" s="10" t="str">
+      <c r="M56" s="1"/>
+      <c r="N56" s="10" t="str">
         <f>M9</f>
         <v>Rapaka</v>
       </c>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="10" t="str">
+      <c r="P56" s="1"/>
+      <c r="Q56" s="10" t="str">
         <f>P9</f>
         <v>Sushma</v>
       </c>
-      <c r="S45" s="1"/>
-      <c r="T45" s="10" t="str">
+      <c r="S56" s="1"/>
+      <c r="T56" s="10" t="str">
         <f>S9</f>
         <v>Sampath M</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="6" t="s">
+    <row r="57" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="11">
+      <c r="E57" s="11">
         <f>SUM(D10:D43)</f>
-        <v>-55</v>
-      </c>
-      <c r="G46" s="6" t="s">
+        <v>-75</v>
+      </c>
+      <c r="G57" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H46" s="11">
+      <c r="H57" s="11">
         <f>SUM(G10:G43)</f>
-        <v>-82.5</v>
-      </c>
-      <c r="J46" s="6" t="s">
+        <v>-107.5</v>
+      </c>
+      <c r="J57" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K46" s="11">
+      <c r="K57" s="11">
         <f>SUM(J10:J43)</f>
-        <v>-25</v>
-      </c>
-      <c r="M46" s="6" t="s">
+        <v>-35</v>
+      </c>
+      <c r="M57" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N46" s="11">
+      <c r="N57" s="11">
         <f>SUM(M10:M43)</f>
-        <v>85</v>
-      </c>
-      <c r="P46" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="P57" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q46" s="11">
+      <c r="Q57" s="11">
         <f>SUM(P10:P43)</f>
         <v>85</v>
       </c>
-      <c r="S46" s="6" t="s">
+      <c r="S57" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="T46" s="11">
+      <c r="T57" s="11">
         <f>SUM(S10:S43)</f>
-        <v>-7.5</v>
-      </c>
-      <c r="U46" s="1">
-        <f>SUM(E46,H46,K46,N46,Q46,T46)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
+        <v>7.5</v>
+      </c>
+      <c r="U57" s="1">
+        <f>SUM(E57,H57,K57,N57,Q57,T57)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3163,7 +3461,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E46">
+  <conditionalFormatting sqref="E57">
     <cfRule type="cellIs" dxfId="17" priority="91" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3174,7 +3472,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H46">
+  <conditionalFormatting sqref="H57">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3185,7 +3483,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K46">
+  <conditionalFormatting sqref="K57">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3196,7 +3494,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N46">
+  <conditionalFormatting sqref="N57">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3207,7 +3505,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q46">
+  <conditionalFormatting sqref="Q57">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3218,7 +3516,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T46">
+  <conditionalFormatting sqref="T57">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Contest 35 RCB vs CSK.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659CEE97-21A9-9146-A8F5-65BDA40794F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A97E19-ECA2-CF4F-8FAF-2EF68D6BBF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="4000" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -572,7 +572,157 @@
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3070,18 +3220,48 @@
       <c r="C44" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="1"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="1"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="1"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="1"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="1"/>
-      <c r="S44" s="3"/>
-      <c r="T44" s="1"/>
+      <c r="D44" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(E44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$C$7, $B44+1, FALSE)),"",VLOOKUP(RANK(E44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$C$7, $B44+1, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="E44" s="1">
+        <v>60</v>
+      </c>
+      <c r="G44" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$C$7, $B44+1, FALSE)),"",VLOOKUP(RANK(H44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$C$7, $B44+1, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="H44" s="1">
+        <v>40</v>
+      </c>
+      <c r="J44" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$C$7, $B44+1, FALSE)),"",VLOOKUP(RANK(K44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$C$7, $B44+1, FALSE))</f>
+        <v>40</v>
+      </c>
+      <c r="K44" s="1">
+        <v>100</v>
+      </c>
+      <c r="M44" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$C$7, $B44+1, FALSE)),"",VLOOKUP(RANK(N44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$C$7, $B44+1, FALSE))</f>
+        <v>15</v>
+      </c>
+      <c r="N44" s="1">
+        <v>80</v>
+      </c>
+      <c r="P44" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$C$7, $B44+1, FALSE)),"",VLOOKUP(RANK(Q44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$C$7, $B44+1, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>0</v>
+      </c>
+      <c r="S44" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$C$7, $B44+1, FALSE)),"",VLOOKUP(RANK(T44, ($T44,$Q44,$N44,$K44,$H44,$E44), 0),  $A$2:$C$7, $B44+1, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="T44" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
@@ -3093,17 +3273,35 @@
       <c r="C45" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D45" s="3"/>
+      <c r="D45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE)),"",VLOOKUP(RANK(E45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="E45" s="1"/>
-      <c r="G45" s="3"/>
+      <c r="G45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE)),"",VLOOKUP(RANK(H45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="H45" s="1"/>
-      <c r="J45" s="3"/>
+      <c r="J45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE)),"",VLOOKUP(RANK(K45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="K45" s="1"/>
-      <c r="M45" s="3"/>
+      <c r="M45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE)),"",VLOOKUP(RANK(N45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="N45" s="1"/>
-      <c r="P45" s="3"/>
+      <c r="P45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE)),"",VLOOKUP(RANK(Q45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q45" s="1"/>
-      <c r="S45" s="3"/>
+      <c r="S45" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE)),"",VLOOKUP(RANK(T45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="T45" s="1"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
@@ -3116,17 +3314,35 @@
       <c r="C46" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE)),"",VLOOKUP(RANK(E46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="E46" s="1"/>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE)),"",VLOOKUP(RANK(H46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="H46" s="1"/>
-      <c r="J46" s="3"/>
+      <c r="J46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE)),"",VLOOKUP(RANK(K46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="K46" s="1"/>
-      <c r="M46" s="3"/>
+      <c r="M46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE)),"",VLOOKUP(RANK(N46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="N46" s="1"/>
-      <c r="P46" s="3"/>
+      <c r="P46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE)),"",VLOOKUP(RANK(Q46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q46" s="1"/>
-      <c r="S46" s="3"/>
+      <c r="S46" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE)),"",VLOOKUP(RANK(T46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="T46" s="1"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
@@ -3139,17 +3355,35 @@
       <c r="C47" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D47" s="3"/>
+      <c r="D47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE)),"",VLOOKUP(RANK(E47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="E47" s="1"/>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE)),"",VLOOKUP(RANK(H47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="H47" s="1"/>
-      <c r="J47" s="3"/>
+      <c r="J47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE)),"",VLOOKUP(RANK(K47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="K47" s="1"/>
-      <c r="M47" s="3"/>
+      <c r="M47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE)),"",VLOOKUP(RANK(N47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="N47" s="1"/>
-      <c r="P47" s="3"/>
+      <c r="P47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE)),"",VLOOKUP(RANK(Q47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q47" s="1"/>
-      <c r="S47" s="3"/>
+      <c r="S47" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE)),"",VLOOKUP(RANK(T47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="T47" s="1"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
@@ -3162,17 +3396,35 @@
       <c r="C48" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="3"/>
+      <c r="D48" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE)),"",VLOOKUP(RANK(E48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="E48" s="1"/>
-      <c r="G48" s="3"/>
+      <c r="G48" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE)),"",VLOOKUP(RANK(H48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="H48" s="1"/>
-      <c r="J48" s="3"/>
+      <c r="J48" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE)),"",VLOOKUP(RANK(K48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="K48" s="1"/>
-      <c r="M48" s="3"/>
+      <c r="M48" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE)),"",VLOOKUP(RANK(N48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="N48" s="1"/>
-      <c r="P48" s="3"/>
+      <c r="P48" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE)),"",VLOOKUP(RANK(Q48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q48" s="1"/>
-      <c r="S48" s="3"/>
+      <c r="S48" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE)),"",VLOOKUP(RANK(T48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="T48" s="1"/>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
@@ -3185,17 +3437,35 @@
       <c r="C49" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D49" s="3"/>
+      <c r="D49" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE)),"",VLOOKUP(RANK(E49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="E49" s="1"/>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE)),"",VLOOKUP(RANK(H49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="H49" s="1"/>
-      <c r="J49" s="3"/>
+      <c r="J49" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE)),"",VLOOKUP(RANK(K49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="K49" s="1"/>
-      <c r="M49" s="3"/>
+      <c r="M49" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE)),"",VLOOKUP(RANK(N49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="N49" s="1"/>
-      <c r="P49" s="3"/>
+      <c r="P49" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE)),"",VLOOKUP(RANK(Q49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q49" s="1"/>
-      <c r="S49" s="3"/>
+      <c r="S49" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE)),"",VLOOKUP(RANK(T49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="T49" s="1"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
@@ -3208,17 +3478,35 @@
       <c r="C50" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="3"/>
+      <c r="D50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE)),"",VLOOKUP(RANK(E50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="E50" s="1"/>
-      <c r="G50" s="3"/>
+      <c r="G50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE)),"",VLOOKUP(RANK(H50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="H50" s="1"/>
-      <c r="J50" s="3"/>
+      <c r="J50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE)),"",VLOOKUP(RANK(K50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="K50" s="1"/>
-      <c r="M50" s="3"/>
+      <c r="M50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE)),"",VLOOKUP(RANK(N50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="N50" s="1"/>
-      <c r="P50" s="3"/>
+      <c r="P50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE)),"",VLOOKUP(RANK(Q50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q50" s="1"/>
-      <c r="S50" s="3"/>
+      <c r="S50" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE)),"",VLOOKUP(RANK(T50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="T50" s="1"/>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.2">
@@ -3231,17 +3519,35 @@
       <c r="C51" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="D51" s="3"/>
+      <c r="D51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE)),"",VLOOKUP(RANK(E51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="E51" s="1"/>
-      <c r="G51" s="3"/>
+      <c r="G51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE)),"",VLOOKUP(RANK(H51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="H51" s="1"/>
-      <c r="J51" s="3"/>
+      <c r="J51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE)),"",VLOOKUP(RANK(K51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="K51" s="1"/>
-      <c r="M51" s="3"/>
+      <c r="M51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE)),"",VLOOKUP(RANK(N51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="N51" s="1"/>
-      <c r="P51" s="3"/>
+      <c r="P51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE)),"",VLOOKUP(RANK(Q51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q51" s="1"/>
-      <c r="S51" s="3"/>
+      <c r="S51" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE)),"",VLOOKUP(RANK(T51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="T51" s="1"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.2">
@@ -3254,17 +3560,35 @@
       <c r="C52" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D52" s="3"/>
+      <c r="D52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE)),"",VLOOKUP(RANK(E52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="E52" s="1"/>
-      <c r="G52" s="3"/>
+      <c r="G52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE)),"",VLOOKUP(RANK(H52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="H52" s="1"/>
-      <c r="J52" s="3"/>
+      <c r="J52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE)),"",VLOOKUP(RANK(K52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="K52" s="1"/>
-      <c r="M52" s="3"/>
+      <c r="M52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE)),"",VLOOKUP(RANK(N52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="N52" s="1"/>
-      <c r="P52" s="3"/>
+      <c r="P52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE)),"",VLOOKUP(RANK(Q52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q52" s="1"/>
-      <c r="S52" s="3"/>
+      <c r="S52" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE)),"",VLOOKUP(RANK(T52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="T52" s="1"/>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
@@ -3277,17 +3601,35 @@
       <c r="C53" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="D53" s="3"/>
+      <c r="D53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE)),"",VLOOKUP(RANK(E53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="E53" s="1"/>
-      <c r="G53" s="3"/>
+      <c r="G53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE)),"",VLOOKUP(RANK(H53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="H53" s="1"/>
-      <c r="J53" s="3"/>
+      <c r="J53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE)),"",VLOOKUP(RANK(K53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="K53" s="1"/>
-      <c r="M53" s="3"/>
+      <c r="M53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE)),"",VLOOKUP(RANK(N53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="N53" s="1"/>
-      <c r="P53" s="3"/>
+      <c r="P53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE)),"",VLOOKUP(RANK(Q53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q53" s="1"/>
-      <c r="S53" s="3"/>
+      <c r="S53" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE)),"",VLOOKUP(RANK(T53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="T53" s="1"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">
@@ -3300,17 +3642,35 @@
       <c r="C54" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="D54" s="3"/>
+      <c r="D54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE)),"",VLOOKUP(RANK(E54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="E54" s="1"/>
-      <c r="G54" s="3"/>
+      <c r="G54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE)),"",VLOOKUP(RANK(H54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="H54" s="1"/>
-      <c r="J54" s="3"/>
+      <c r="J54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE)),"",VLOOKUP(RANK(K54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="K54" s="1"/>
-      <c r="M54" s="3"/>
+      <c r="M54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE)),"",VLOOKUP(RANK(N54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="N54" s="1"/>
-      <c r="P54" s="3"/>
+      <c r="P54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE)),"",VLOOKUP(RANK(Q54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="Q54" s="1"/>
-      <c r="S54" s="3"/>
+      <c r="S54" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE)),"",VLOOKUP(RANK(T54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE))</f>
+        <v/>
+      </c>
       <c r="T54" s="1"/>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.2">
@@ -3387,43 +3747,43 @@
         <v>12</v>
       </c>
       <c r="E57" s="11">
-        <f>SUM(D10:D43)</f>
-        <v>-75</v>
+        <f>SUM(D10:D54)</f>
+        <v>-85</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H57" s="11">
-        <f>SUM(G10:G43)</f>
-        <v>-107.5</v>
+        <f>SUM(G10:G54)</f>
+        <v>-127.5</v>
       </c>
       <c r="J57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K57" s="11">
-        <f>SUM(J10:J43)</f>
-        <v>-35</v>
+        <f>SUM(J10:J54)</f>
+        <v>5</v>
       </c>
       <c r="M57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N57" s="11">
-        <f>SUM(M10:M43)</f>
-        <v>125</v>
+        <f>SUM(M10:M54)</f>
+        <v>140</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q57" s="11">
-        <f>SUM(P10:P43)</f>
+        <f>SUM(P10:P54)</f>
         <v>85</v>
       </c>
       <c r="S57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T57" s="11">
-        <f>SUM(S10:S43)</f>
-        <v>7.5</v>
+        <f>SUM(S10:S54)</f>
+        <v>-17.5</v>
       </c>
       <c r="U57" s="1">
         <f>SUM(E57,H57,K57,N57,Q57,T57)</f>
@@ -3462,13 +3822,13 @@
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
   <conditionalFormatting sqref="E57">
-    <cfRule type="cellIs" dxfId="17" priority="91" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="106" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="107" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="93" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="108" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Contest 36 DC vs RR & Contest 37 SRH vs PBKS
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A97E19-ECA2-CF4F-8FAF-2EF68D6BBF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0728946B-5A58-354C-840F-246D7FAE8BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="4000" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="760" yWindow="3980" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3273,36 +3273,48 @@
       <c r="C45" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D45" s="3" t="str">
+      <c r="D45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE)),"",VLOOKUP(RANK(E45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E45" s="1"/>
-      <c r="G45" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E45" s="1">
+        <v>60</v>
+      </c>
+      <c r="G45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE)),"",VLOOKUP(RANK(H45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H45" s="1"/>
-      <c r="J45" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="H45" s="1">
+        <v>100</v>
+      </c>
+      <c r="J45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE)),"",VLOOKUP(RANK(K45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K45" s="1"/>
-      <c r="M45" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K45" s="1">
+        <v>40</v>
+      </c>
+      <c r="M45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE)),"",VLOOKUP(RANK(N45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N45" s="1"/>
-      <c r="P45" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N45" s="1">
+        <v>20</v>
+      </c>
+      <c r="P45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE)),"",VLOOKUP(RANK(Q45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q45" s="1"/>
-      <c r="S45" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>0</v>
+      </c>
+      <c r="S45" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE)),"",VLOOKUP(RANK(T45, ($T45,$Q45,$N45,$K45,$H45,$E45), 0),  $A$2:$C$7, $B45+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T45" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="T45" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
@@ -3314,36 +3326,48 @@
       <c r="C46" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D46" s="3" t="str">
+      <c r="D46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE)),"",VLOOKUP(RANK(E46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E46" s="1"/>
-      <c r="G46" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="E46" s="1">
+        <v>100</v>
+      </c>
+      <c r="G46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE)),"",VLOOKUP(RANK(H46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H46" s="1"/>
-      <c r="J46" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H46" s="1">
+        <v>40</v>
+      </c>
+      <c r="J46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE)),"",VLOOKUP(RANK(K46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K46" s="1"/>
-      <c r="M46" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K46" s="1">
+        <v>60</v>
+      </c>
+      <c r="M46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE)),"",VLOOKUP(RANK(N46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N46" s="1"/>
-      <c r="P46" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N46" s="1">
+        <v>20</v>
+      </c>
+      <c r="P46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE)),"",VLOOKUP(RANK(Q46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q46" s="1"/>
-      <c r="S46" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>0</v>
+      </c>
+      <c r="S46" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE)),"",VLOOKUP(RANK(T46, ($T46,$Q46,$N46,$K46,$H46,$E46), 0),  $A$2:$C$7, $B46+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T46" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="T46" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
@@ -3748,28 +3772,28 @@
       </c>
       <c r="E57" s="11">
         <f>SUM(D10:D54)</f>
-        <v>-85</v>
+        <v>-55</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H57" s="11">
         <f>SUM(G10:G54)</f>
-        <v>-127.5</v>
+        <v>-107.5</v>
       </c>
       <c r="J57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K57" s="11">
         <f>SUM(J10:J54)</f>
-        <v>5</v>
+        <v>-25</v>
       </c>
       <c r="M57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N57" s="11">
         <f>SUM(M10:M54)</f>
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>12</v>
@@ -3783,7 +3807,7 @@
       </c>
       <c r="T57" s="11">
         <f>SUM(S10:S54)</f>
-        <v>-17.5</v>
+        <v>12.5</v>
       </c>
       <c r="U57" s="1">
         <f>SUM(E57,H57,K57,N57,Q57,T57)</f>

</xml_diff>

<commit_message>
Contest 38 CSK vs KKR & Contest 39 RCB vs MI.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0728946B-5A58-354C-840F-246D7FAE8BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3833F3C1-4BC1-8D44-91CD-D1E4A7A2941B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="3980" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -3379,36 +3379,48 @@
       <c r="C47" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D47" s="3" t="str">
+      <c r="D47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE)),"",VLOOKUP(RANK(E47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E47" s="1"/>
-      <c r="G47" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E47" s="1">
+        <v>60</v>
+      </c>
+      <c r="G47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE)),"",VLOOKUP(RANK(H47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H47" s="1"/>
-      <c r="J47" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="H47" s="1">
+        <v>100</v>
+      </c>
+      <c r="J47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE)),"",VLOOKUP(RANK(K47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K47" s="1"/>
-      <c r="M47" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K47" s="1">
+        <v>20</v>
+      </c>
+      <c r="M47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE)),"",VLOOKUP(RANK(N47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N47" s="1"/>
-      <c r="P47" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N47" s="1">
+        <v>40</v>
+      </c>
+      <c r="P47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE)),"",VLOOKUP(RANK(Q47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q47" s="1"/>
-      <c r="S47" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>0</v>
+      </c>
+      <c r="S47" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE)),"",VLOOKUP(RANK(T47, ($T47,$Q47,$N47,$K47,$H47,$E47), 0),  $A$2:$C$7, $B47+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T47" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="T47" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
@@ -3420,36 +3432,48 @@
       <c r="C48" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="3" t="str">
+      <c r="D48" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE)),"",VLOOKUP(RANK(E48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E48" s="1"/>
-      <c r="G48" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="E48" s="1">
+        <v>100</v>
+      </c>
+      <c r="G48" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE)),"",VLOOKUP(RANK(H48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H48" s="1"/>
-      <c r="J48" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H48" s="1">
+        <v>60</v>
+      </c>
+      <c r="J48" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE)),"",VLOOKUP(RANK(K48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K48" s="1"/>
-      <c r="M48" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="K48" s="1">
+        <v>80</v>
+      </c>
+      <c r="M48" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE)),"",VLOOKUP(RANK(N48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N48" s="1"/>
-      <c r="P48" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N48" s="1">
+        <v>40</v>
+      </c>
+      <c r="P48" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE)),"",VLOOKUP(RANK(Q48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q48" s="1"/>
-      <c r="S48" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>0</v>
+      </c>
+      <c r="S48" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE)),"",VLOOKUP(RANK(T48, ($T48,$Q48,$N48,$K48,$H48,$E48), 0),  $A$2:$C$7, $B48+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T48" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T48" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
@@ -3772,28 +3796,28 @@
       </c>
       <c r="E57" s="11">
         <f>SUM(D10:D54)</f>
-        <v>-55</v>
+        <v>-25</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H57" s="11">
         <f>SUM(G10:G54)</f>
-        <v>-107.5</v>
+        <v>-77.5</v>
       </c>
       <c r="J57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K57" s="11">
         <f>SUM(J10:J54)</f>
-        <v>-25</v>
+        <v>-35</v>
       </c>
       <c r="M57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N57" s="11">
         <f>SUM(M10:M54)</f>
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>12</v>
@@ -3807,7 +3831,7 @@
       </c>
       <c r="T57" s="11">
         <f>SUM(S10:S54)</f>
-        <v>12.5</v>
+        <v>2.5</v>
       </c>
       <c r="U57" s="1">
         <f>SUM(E57,H57,K57,N57,Q57,T57)</f>

</xml_diff>

<commit_message>
Contest 40 SRH vs RR.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3833F3C1-4BC1-8D44-91CD-D1E4A7A2941B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D57516-C471-044C-ACAC-55A5845C1166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="3980" windowWidth="30160" windowHeight="16640" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="2500" yWindow="2360" windowWidth="30320" windowHeight="17120" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3485,36 +3485,48 @@
       <c r="C49" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D49" s="3" t="str">
+      <c r="D49" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE)),"",VLOOKUP(RANK(E49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E49" s="1"/>
-      <c r="G49" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="E49" s="1">
+        <v>80</v>
+      </c>
+      <c r="G49" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE)),"",VLOOKUP(RANK(H49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H49" s="1"/>
-      <c r="J49" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H49" s="1">
+        <v>60</v>
+      </c>
+      <c r="J49" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE)),"",VLOOKUP(RANK(K49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K49" s="1"/>
-      <c r="M49" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K49" s="1">
+        <v>40</v>
+      </c>
+      <c r="M49" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE)),"",VLOOKUP(RANK(N49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N49" s="1"/>
-      <c r="P49" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="N49" s="1">
+        <v>100</v>
+      </c>
+      <c r="P49" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE)),"",VLOOKUP(RANK(Q49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q49" s="1"/>
-      <c r="S49" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>0</v>
+      </c>
+      <c r="S49" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE)),"",VLOOKUP(RANK(T49, ($T49,$Q49,$N49,$K49,$H49,$E49), 0),  $A$2:$C$7, $B49+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T49" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T49" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
@@ -3796,28 +3808,28 @@
       </c>
       <c r="E57" s="11">
         <f>SUM(D10:D54)</f>
-        <v>-25</v>
+        <v>-10</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H57" s="11">
         <f>SUM(G10:G54)</f>
-        <v>-77.5</v>
+        <v>-87.5</v>
       </c>
       <c r="J57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K57" s="11">
         <f>SUM(J10:J54)</f>
-        <v>-35</v>
+        <v>-55</v>
       </c>
       <c r="M57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N57" s="11">
         <f>SUM(M10:M54)</f>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>12</v>
@@ -3831,7 +3843,7 @@
       </c>
       <c r="T57" s="11">
         <f>SUM(S10:S54)</f>
-        <v>2.5</v>
+        <v>-22.5</v>
       </c>
       <c r="U57" s="1">
         <f>SUM(E57,H57,K57,N57,Q57,T57)</f>

</xml_diff>

<commit_message>
Contest 41 KKR vs DC & Contest 42 MI vs PBKS.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D57516-C471-044C-ACAC-55A5845C1166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4B8824-8E55-7246-818E-958784B17889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="2360" windowWidth="30320" windowHeight="17120" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -3538,36 +3538,48 @@
       <c r="C50" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="D50" s="3" t="str">
+      <c r="D50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE)),"",VLOOKUP(RANK(E50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E50" s="1"/>
-      <c r="G50" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E50" s="1">
+        <v>60</v>
+      </c>
+      <c r="G50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE)),"",VLOOKUP(RANK(H50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H50" s="1"/>
-      <c r="J50" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H50" s="1">
+        <v>40</v>
+      </c>
+      <c r="J50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE)),"",VLOOKUP(RANK(K50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K50" s="1"/>
-      <c r="M50" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="K50" s="1">
+        <v>80</v>
+      </c>
+      <c r="M50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE)),"",VLOOKUP(RANK(N50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N50" s="1"/>
-      <c r="P50" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N50" s="1">
+        <v>20</v>
+      </c>
+      <c r="P50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE)),"",VLOOKUP(RANK(Q50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q50" s="1"/>
-      <c r="S50" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>0</v>
+      </c>
+      <c r="S50" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE)),"",VLOOKUP(RANK(T50, ($T50,$Q50,$N50,$K50,$H50,$E50), 0),  $A$2:$C$7, $B50+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T50" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="T50" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
@@ -3579,36 +3591,48 @@
       <c r="C51" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="D51" s="3" t="str">
+      <c r="D51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE)),"",VLOOKUP(RANK(E51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E51" s="1"/>
-      <c r="G51" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="E51" s="1">
+        <v>80</v>
+      </c>
+      <c r="G51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE)),"",VLOOKUP(RANK(H51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H51" s="1"/>
-      <c r="J51" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H51" s="1">
+        <v>20</v>
+      </c>
+      <c r="J51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE)),"",VLOOKUP(RANK(K51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K51" s="1"/>
-      <c r="M51" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K51" s="1">
+        <v>60</v>
+      </c>
+      <c r="M51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE)),"",VLOOKUP(RANK(N51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N51" s="1"/>
-      <c r="P51" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="N51" s="1">
+        <v>100</v>
+      </c>
+      <c r="P51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE)),"",VLOOKUP(RANK(Q51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q51" s="1"/>
-      <c r="S51" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>0</v>
+      </c>
+      <c r="S51" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE)),"",VLOOKUP(RANK(T51, ($T51,$Q51,$N51,$K51,$H51,$E51), 0),  $A$2:$C$7, $B51+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T51" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="T51" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
@@ -3808,28 +3832,28 @@
       </c>
       <c r="E57" s="11">
         <f>SUM(D10:D54)</f>
-        <v>-10</v>
+        <v>-5</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H57" s="11">
         <f>SUM(G10:G54)</f>
-        <v>-87.5</v>
+        <v>-132.5</v>
       </c>
       <c r="J57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K57" s="11">
         <f>SUM(J10:J54)</f>
-        <v>-55</v>
+        <v>-50</v>
       </c>
       <c r="M57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N57" s="11">
         <f>SUM(M10:M54)</f>
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>12</v>
@@ -3843,7 +3867,7 @@
       </c>
       <c r="T57" s="11">
         <f>SUM(S10:S54)</f>
-        <v>-22.5</v>
+        <v>-2.5</v>
       </c>
       <c r="U57" s="1">
         <f>SUM(E57,H57,K57,N57,Q57,T57)</f>

</xml_diff>

<commit_message>
Contest 43 RR vs RCB.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4B8824-8E55-7246-818E-958784B17889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89F5F1F-6DAE-A54A-A499-9AB118907D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="2360" windowWidth="30320" windowHeight="17120" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -3644,36 +3644,48 @@
       <c r="C52" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D52" s="3" t="str">
+      <c r="D52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE)),"",VLOOKUP(RANK(E52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E52" s="1"/>
-      <c r="G52" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="E52" s="1">
+        <v>80</v>
+      </c>
+      <c r="G52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE)),"",VLOOKUP(RANK(H52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H52" s="1"/>
-      <c r="J52" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H52" s="1">
+        <v>60</v>
+      </c>
+      <c r="J52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE)),"",VLOOKUP(RANK(K52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K52" s="1"/>
-      <c r="M52" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K52" s="1">
+        <v>20</v>
+      </c>
+      <c r="M52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE)),"",VLOOKUP(RANK(N52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N52" s="1"/>
-      <c r="P52" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N52" s="1">
+        <v>40</v>
+      </c>
+      <c r="P52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE)),"",VLOOKUP(RANK(Q52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q52" s="1"/>
-      <c r="S52" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>0</v>
+      </c>
+      <c r="S52" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE)),"",VLOOKUP(RANK(T52, ($T52,$Q52,$N52,$K52,$H52,$E52), 0),  $A$2:$C$7, $B52+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T52" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="T52" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
@@ -3832,28 +3844,28 @@
       </c>
       <c r="E57" s="11">
         <f>SUM(D10:D54)</f>
-        <v>-5</v>
+        <v>10</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H57" s="11">
         <f>SUM(G10:G54)</f>
-        <v>-132.5</v>
+        <v>-142.5</v>
       </c>
       <c r="J57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K57" s="11">
         <f>SUM(J10:J54)</f>
-        <v>-50</v>
+        <v>-75</v>
       </c>
       <c r="M57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N57" s="11">
         <f>SUM(M10:M54)</f>
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>12</v>
@@ -3867,7 +3879,7 @@
       </c>
       <c r="T57" s="11">
         <f>SUM(S10:S54)</f>
-        <v>-2.5</v>
+        <v>37.5</v>
       </c>
       <c r="U57" s="1">
         <f>SUM(E57,H57,K57,N57,Q57,T57)</f>

</xml_diff>

<commit_message>
Contest 44 SRH vs CSK.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89F5F1F-6DAE-A54A-A499-9AB118907D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C6C93D-C02E-C845-B329-94ED5147181F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="2360" windowWidth="30320" windowHeight="17120" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -3697,36 +3697,48 @@
       <c r="C53" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="D53" s="3" t="str">
+      <c r="D53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE)),"",VLOOKUP(RANK(E53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E53" s="1"/>
-      <c r="G53" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="E53" s="1">
+        <v>80</v>
+      </c>
+      <c r="G53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE)),"",VLOOKUP(RANK(H53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H53" s="1"/>
-      <c r="J53" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H53" s="1">
+        <v>60</v>
+      </c>
+      <c r="J53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE)),"",VLOOKUP(RANK(K53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K53" s="1"/>
-      <c r="M53" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="K53" s="1">
+        <v>100</v>
+      </c>
+      <c r="M53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE)),"",VLOOKUP(RANK(N53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N53" s="1"/>
-      <c r="P53" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N53" s="1">
+        <v>20</v>
+      </c>
+      <c r="P53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE)),"",VLOOKUP(RANK(Q53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q53" s="1"/>
-      <c r="S53" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>0</v>
+      </c>
+      <c r="S53" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE)),"",VLOOKUP(RANK(T53, ($T53,$Q53,$N53,$K53,$H53,$E53), 0),  $A$2:$C$7, $B53+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T53" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="T53" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
@@ -3844,28 +3856,28 @@
       </c>
       <c r="E57" s="11">
         <f>SUM(D10:D54)</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H57" s="11">
         <f>SUM(G10:G54)</f>
-        <v>-142.5</v>
+        <v>-152.5</v>
       </c>
       <c r="J57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K57" s="11">
         <f>SUM(J10:J54)</f>
-        <v>-75</v>
+        <v>-35</v>
       </c>
       <c r="M57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N57" s="11">
         <f>SUM(M10:M54)</f>
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>12</v>
@@ -3879,7 +3891,7 @@
       </c>
       <c r="T57" s="11">
         <f>SUM(S10:S54)</f>
-        <v>37.5</v>
+        <v>17.5</v>
       </c>
       <c r="U57" s="1">
         <f>SUM(E57,H57,K57,N57,Q57,T57)</f>

</xml_diff>

<commit_message>
Contest 45 KKR vs PBKS.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C6C93D-C02E-C845-B329-94ED5147181F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B3000D-709C-C049-8EC9-15EA29F36DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="2360" windowWidth="30320" windowHeight="17120" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -3750,36 +3750,48 @@
       <c r="C54" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="D54" s="3" t="str">
+      <c r="D54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE)),"",VLOOKUP(RANK(E54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E54" s="1"/>
-      <c r="G54" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="E54" s="1">
+        <v>80</v>
+      </c>
+      <c r="G54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE)),"",VLOOKUP(RANK(H54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H54" s="1"/>
-      <c r="J54" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="H54" s="1">
+        <v>100</v>
+      </c>
+      <c r="J54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE)),"",VLOOKUP(RANK(K54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K54" s="1"/>
-      <c r="M54" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K54" s="1">
+        <v>60</v>
+      </c>
+      <c r="M54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE)),"",VLOOKUP(RANK(N54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N54" s="1"/>
-      <c r="P54" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N54" s="1">
+        <v>40</v>
+      </c>
+      <c r="P54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE)),"",VLOOKUP(RANK(Q54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q54" s="1"/>
-      <c r="S54" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="1">
+        <v>0</v>
+      </c>
+      <c r="S54" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE)),"",VLOOKUP(RANK(T54, ($T54,$Q54,$N54,$K54,$H54,$E54), 0),  $A$2:$C$7, $B54+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T54" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T54" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" s="5"/>
@@ -3856,28 +3868,28 @@
       </c>
       <c r="E57" s="11">
         <f>SUM(D10:D54)</f>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H57" s="11">
         <f>SUM(G10:G54)</f>
-        <v>-152.5</v>
+        <v>-112.5</v>
       </c>
       <c r="J57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K57" s="11">
         <f>SUM(J10:J54)</f>
-        <v>-35</v>
+        <v>-45</v>
       </c>
       <c r="M57" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N57" s="11">
         <f>SUM(M10:M54)</f>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>12</v>
@@ -3891,7 +3903,7 @@
       </c>
       <c r="T57" s="11">
         <f>SUM(S10:S54)</f>
-        <v>17.5</v>
+        <v>-7.5</v>
       </c>
       <c r="U57" s="1">
         <f>SUM(E57,H57,K57,N57,Q57,T57)</f>

</xml_diff>

<commit_message>
Added rest of the leage schedule.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B3000D-709C-C049-8EC9-15EA29F36DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FEF871-0EDE-554F-A964-5CD3BDB67DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="2360" windowWidth="30320" windowHeight="17120" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="98">
   <si>
     <t>Points</t>
   </si>
@@ -293,6 +293,39 @@
   </si>
   <si>
     <t>KKR vs PBKS</t>
+  </si>
+  <si>
+    <t>MI vs DC</t>
+  </si>
+  <si>
+    <t>RR vs CSK</t>
+  </si>
+  <si>
+    <t>RCB vs PBKS</t>
+  </si>
+  <si>
+    <t>KKR vs SRH</t>
+  </si>
+  <si>
+    <t>DC vs CSK</t>
+  </si>
+  <si>
+    <t>RR vs MI</t>
+  </si>
+  <si>
+    <t>RCB vs SRH</t>
+  </si>
+  <si>
+    <t>CSK vs PBKS</t>
+  </si>
+  <si>
+    <t>KKR vs RR</t>
+  </si>
+  <si>
+    <t>SRH vs MI</t>
+  </si>
+  <si>
+    <t>RCB vs DC</t>
   </si>
 </sst>
 </file>
@@ -1213,11 +1246,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U60"/>
+  <dimension ref="A1:U71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U57" sqref="U57"/>
+      <pane ySplit="8" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U68" sqref="U68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3475,7 +3508,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>40</v>
       </c>
@@ -3528,7 +3561,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>41</v>
       </c>
@@ -3581,7 +3614,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>42</v>
       </c>
@@ -3634,7 +3667,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43</v>
       </c>
@@ -3687,7 +3720,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>44</v>
       </c>
@@ -3740,7 +3773,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <v>45</v>
       </c>
@@ -3793,143 +3826,594 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A55" s="5"/>
-      <c r="B55" s="1" t="s">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>46</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE)),"",VLOOKUP(RANK(E55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E55" s="1"/>
+      <c r="G55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE)),"",VLOOKUP(RANK(H55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H55" s="1"/>
+      <c r="J55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE)),"",VLOOKUP(RANK(K55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K55" s="1"/>
+      <c r="M55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE)),"",VLOOKUP(RANK(N55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N55" s="1"/>
+      <c r="P55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE)),"",VLOOKUP(RANK(Q55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q55" s="1"/>
+      <c r="S55" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE)),"",VLOOKUP(RANK(T55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T55" s="1"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
+        <v>47</v>
+      </c>
+      <c r="B56" s="1">
+        <v>2</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE)),"",VLOOKUP(RANK(E56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="G56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE)),"",VLOOKUP(RANK(H56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H56" s="1"/>
+      <c r="J56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE)),"",VLOOKUP(RANK(K56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K56" s="1"/>
+      <c r="M56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE)),"",VLOOKUP(RANK(N56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N56" s="1"/>
+      <c r="P56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE)),"",VLOOKUP(RANK(Q56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q56" s="1"/>
+      <c r="S56" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE)),"",VLOOKUP(RANK(T56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T56" s="1"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>48</v>
+      </c>
+      <c r="B57" s="1">
+        <v>2</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE)),"",VLOOKUP(RANK(E57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="G57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE)),"",VLOOKUP(RANK(H57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H57" s="1"/>
+      <c r="J57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE)),"",VLOOKUP(RANK(K57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K57" s="1"/>
+      <c r="M57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE)),"",VLOOKUP(RANK(N57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N57" s="1"/>
+      <c r="P57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE)),"",VLOOKUP(RANK(Q57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q57" s="1"/>
+      <c r="S57" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE)),"",VLOOKUP(RANK(T57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T57" s="1"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A58" s="5">
+        <v>49</v>
+      </c>
+      <c r="B58" s="1">
+        <v>2</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE)),"",VLOOKUP(RANK(E58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E58" s="1"/>
+      <c r="G58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE)),"",VLOOKUP(RANK(H58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H58" s="1"/>
+      <c r="J58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE)),"",VLOOKUP(RANK(K58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K58" s="1"/>
+      <c r="M58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE)),"",VLOOKUP(RANK(N58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N58" s="1"/>
+      <c r="P58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE)),"",VLOOKUP(RANK(Q58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q58" s="1"/>
+      <c r="S58" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE)),"",VLOOKUP(RANK(T58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T58" s="1"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>50</v>
+      </c>
+      <c r="B59" s="1">
+        <v>2</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE)),"",VLOOKUP(RANK(E59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="G59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE)),"",VLOOKUP(RANK(H59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H59" s="1"/>
+      <c r="J59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE)),"",VLOOKUP(RANK(K59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K59" s="1"/>
+      <c r="M59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE)),"",VLOOKUP(RANK(N59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N59" s="1"/>
+      <c r="P59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE)),"",VLOOKUP(RANK(Q59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q59" s="1"/>
+      <c r="S59" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE)),"",VLOOKUP(RANK(T59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T59" s="1"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A60" s="5">
+        <v>51</v>
+      </c>
+      <c r="B60" s="1">
+        <v>2</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE)),"",VLOOKUP(RANK(E60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E60" s="1"/>
+      <c r="G60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE)),"",VLOOKUP(RANK(H60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H60" s="1"/>
+      <c r="J60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE)),"",VLOOKUP(RANK(K60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K60" s="1"/>
+      <c r="M60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE)),"",VLOOKUP(RANK(N60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N60" s="1"/>
+      <c r="P60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE)),"",VLOOKUP(RANK(Q60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q60" s="1"/>
+      <c r="S60" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE)),"",VLOOKUP(RANK(T60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T60" s="1"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>52</v>
+      </c>
+      <c r="B61" s="1">
+        <v>2</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE)),"",VLOOKUP(RANK(E61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="G61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE)),"",VLOOKUP(RANK(H61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H61" s="1"/>
+      <c r="J61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE)),"",VLOOKUP(RANK(K61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K61" s="1"/>
+      <c r="M61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE)),"",VLOOKUP(RANK(N61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N61" s="1"/>
+      <c r="P61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE)),"",VLOOKUP(RANK(Q61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q61" s="1"/>
+      <c r="S61" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE)),"",VLOOKUP(RANK(T61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T61" s="1"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
+        <v>53</v>
+      </c>
+      <c r="B62" s="1">
+        <v>2</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE)),"",VLOOKUP(RANK(E62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="G62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE)),"",VLOOKUP(RANK(H62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H62" s="1"/>
+      <c r="J62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE)),"",VLOOKUP(RANK(K62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K62" s="1"/>
+      <c r="M62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE)),"",VLOOKUP(RANK(N62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N62" s="1"/>
+      <c r="P62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE)),"",VLOOKUP(RANK(Q62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q62" s="1"/>
+      <c r="S62" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE)),"",VLOOKUP(RANK(T62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T62" s="1"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>54</v>
+      </c>
+      <c r="B63" s="1">
+        <v>2</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE)),"",VLOOKUP(RANK(E63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E63" s="1"/>
+      <c r="G63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE)),"",VLOOKUP(RANK(H63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H63" s="1"/>
+      <c r="J63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE)),"",VLOOKUP(RANK(K63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K63" s="1"/>
+      <c r="M63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE)),"",VLOOKUP(RANK(N63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N63" s="1"/>
+      <c r="P63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE)),"",VLOOKUP(RANK(Q63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q63" s="1"/>
+      <c r="S63" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE)),"",VLOOKUP(RANK(T63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T63" s="1"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A64" s="5">
+        <v>55</v>
+      </c>
+      <c r="B64" s="1">
+        <v>2</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE)),"",VLOOKUP(RANK(E64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E64" s="1"/>
+      <c r="G64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE)),"",VLOOKUP(RANK(H64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H64" s="1"/>
+      <c r="J64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE)),"",VLOOKUP(RANK(K64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K64" s="1"/>
+      <c r="M64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE)),"",VLOOKUP(RANK(N64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N64" s="1"/>
+      <c r="P64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE)),"",VLOOKUP(RANK(Q64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q64" s="1"/>
+      <c r="S64" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE)),"",VLOOKUP(RANK(T64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T64" s="1"/>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>56</v>
+      </c>
+      <c r="B65" s="1">
+        <v>2</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(E65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E65" s="1"/>
+      <c r="G65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(H65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H65" s="1"/>
+      <c r="J65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(K65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K65" s="1"/>
+      <c r="M65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(N65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N65" s="1"/>
+      <c r="P65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(Q65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q65" s="1"/>
+      <c r="S65" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(T65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T65" s="1"/>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A66" s="5"/>
+      <c r="B66" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="8" t="s">
+      <c r="C66" s="9"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G55" s="1"/>
-      <c r="H55" s="8" t="s">
+      <c r="G66" s="1"/>
+      <c r="H66" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J55" s="1"/>
-      <c r="K55" s="8" t="s">
+      <c r="J66" s="1"/>
+      <c r="K66" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M55" s="1"/>
-      <c r="N55" s="8" t="s">
+      <c r="M66" s="1"/>
+      <c r="N66" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="8" t="s">
+      <c r="P66" s="1"/>
+      <c r="Q66" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="S55" s="1"/>
-      <c r="T55" s="8" t="s">
+      <c r="S66" s="1"/>
+      <c r="T66" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="10" t="str">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="10" t="str">
         <f>D9</f>
         <v>Anantha</v>
       </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="10" t="str">
+      <c r="G67" s="1"/>
+      <c r="H67" s="10" t="str">
         <f>G9</f>
         <v>Jayanth</v>
       </c>
-      <c r="J56" s="1"/>
-      <c r="K56" s="10" t="str">
+      <c r="J67" s="1"/>
+      <c r="K67" s="10" t="str">
         <f>J9</f>
         <v>Justin</v>
       </c>
-      <c r="M56" s="1"/>
-      <c r="N56" s="10" t="str">
+      <c r="M67" s="1"/>
+      <c r="N67" s="10" t="str">
         <f>M9</f>
         <v>Rapaka</v>
       </c>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="10" t="str">
+      <c r="P67" s="1"/>
+      <c r="Q67" s="10" t="str">
         <f>P9</f>
         <v>Sushma</v>
       </c>
-      <c r="S56" s="1"/>
-      <c r="T56" s="10" t="str">
+      <c r="S67" s="1"/>
+      <c r="T67" s="10" t="str">
         <f>S9</f>
         <v>Sampath M</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="6" t="s">
+    <row r="68" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="11">
+      <c r="E68" s="11">
         <f>SUM(D10:D54)</f>
         <v>40</v>
       </c>
-      <c r="G57" s="6" t="s">
+      <c r="G68" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H57" s="11">
+      <c r="H68" s="11">
         <f>SUM(G10:G54)</f>
         <v>-112.5</v>
       </c>
-      <c r="J57" s="6" t="s">
+      <c r="J68" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K57" s="11">
+      <c r="K68" s="11">
         <f>SUM(J10:J54)</f>
         <v>-45</v>
       </c>
-      <c r="M57" s="6" t="s">
+      <c r="M68" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N57" s="11">
+      <c r="N68" s="11">
         <f>SUM(M10:M54)</f>
         <v>40</v>
       </c>
-      <c r="P57" s="6" t="s">
+      <c r="P68" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q57" s="11">
+      <c r="Q68" s="11">
         <f>SUM(P10:P54)</f>
         <v>85</v>
       </c>
-      <c r="S57" s="6" t="s">
+      <c r="S68" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="T57" s="11">
+      <c r="T68" s="11">
         <f>SUM(S10:S54)</f>
         <v>-7.5</v>
       </c>
-      <c r="U57" s="1">
-        <f>SUM(E57,H57,K57,N57,Q57,T57)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
+      <c r="U68" s="1">
+        <f>SUM(E68,H68,K68,N68,Q68,T68)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3941,7 +4425,7 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E57">
+  <conditionalFormatting sqref="E68">
     <cfRule type="cellIs" dxfId="32" priority="106" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3952,18 +4436,18 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
+  <conditionalFormatting sqref="H68">
+    <cfRule type="cellIs" dxfId="29" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K57">
+  <conditionalFormatting sqref="K68">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3974,7 +4458,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N57">
+  <conditionalFormatting sqref="N68">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3985,7 +4469,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q57">
+  <conditionalFormatting sqref="Q68">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3996,7 +4480,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T57">
+  <conditionalFormatting sqref="T68">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Contest 46 MI vs DC & Contest 47 RR vs CSK.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FEF871-0EDE-554F-A964-5CD3BDB67DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5146CF21-E405-3542-BA36-9745AB2C5B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="2360" windowWidth="30320" windowHeight="17120" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -3836,36 +3836,48 @@
       <c r="C55" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="D55" s="3" t="str">
+      <c r="D55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE)),"",VLOOKUP(RANK(E55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E55" s="1"/>
-      <c r="G55" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E55" s="1">
+        <v>40</v>
+      </c>
+      <c r="G55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE)),"",VLOOKUP(RANK(H55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H55" s="1"/>
-      <c r="J55" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H55" s="1">
+        <v>20</v>
+      </c>
+      <c r="J55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE)),"",VLOOKUP(RANK(K55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K55" s="1"/>
-      <c r="M55" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="K55" s="1">
+        <v>100</v>
+      </c>
+      <c r="M55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE)),"",VLOOKUP(RANK(N55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N55" s="1"/>
-      <c r="P55" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N55" s="1">
+        <v>60</v>
+      </c>
+      <c r="P55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE)),"",VLOOKUP(RANK(Q55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q55" s="1"/>
-      <c r="S55" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="1">
+        <v>0</v>
+      </c>
+      <c r="S55" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE)),"",VLOOKUP(RANK(T55, ($T55,$Q55,$N55,$K55,$H55,$E55), 0),  $A$2:$C$7, $B55+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T55" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="T55" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
@@ -3877,36 +3889,48 @@
       <c r="C56" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="D56" s="3" t="str">
+      <c r="D56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE)),"",VLOOKUP(RANK(E56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E56" s="1"/>
-      <c r="G56" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="E56" s="1">
+        <v>80</v>
+      </c>
+      <c r="G56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE)),"",VLOOKUP(RANK(H56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H56" s="1"/>
-      <c r="J56" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="H56" s="1">
+        <v>100</v>
+      </c>
+      <c r="J56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE)),"",VLOOKUP(RANK(K56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K56" s="1"/>
-      <c r="M56" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K56" s="1">
+        <v>60</v>
+      </c>
+      <c r="M56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE)),"",VLOOKUP(RANK(N56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N56" s="1"/>
-      <c r="P56" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="N56" s="1">
+        <v>20</v>
+      </c>
+      <c r="P56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE)),"",VLOOKUP(RANK(Q56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q56" s="1"/>
-      <c r="S56" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>0</v>
+      </c>
+      <c r="S56" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE)),"",VLOOKUP(RANK(T56, ($T56,$Q56,$N56,$K56,$H56,$E56), 0),  $A$2:$C$7, $B56+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T56" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="T56" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
@@ -4351,43 +4375,43 @@
         <v>12</v>
       </c>
       <c r="E68" s="11">
-        <f>SUM(D10:D54)</f>
-        <v>40</v>
+        <f>SUM(D10:D65)</f>
+        <v>35</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H68" s="11">
-        <f>SUM(G10:G54)</f>
-        <v>-112.5</v>
+        <f>SUM(G10:G65)</f>
+        <v>-97.5</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K68" s="11">
-        <f>SUM(J10:J54)</f>
-        <v>-45</v>
+        <f>SUM(J10:J65)</f>
+        <v>-15</v>
       </c>
       <c r="M68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N68" s="11">
-        <f>SUM(M10:M54)</f>
-        <v>40</v>
+        <f>SUM(M10:M65)</f>
+        <v>5</v>
       </c>
       <c r="P68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="Q68" s="11">
-        <f>SUM(P10:P54)</f>
+        <f>SUM(P10:P65)</f>
         <v>85</v>
       </c>
       <c r="S68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T68" s="11">
-        <f>SUM(S10:S54)</f>
-        <v>-7.5</v>
+        <f>SUM(S10:S65)</f>
+        <v>-12.5</v>
       </c>
       <c r="U68" s="1">
         <f>SUM(E68,H68,K68,N68,Q68,T68)</f>

</xml_diff>

<commit_message>
Contest 48 RCB vs PBKS & Contest 49 KKR vs SRH.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5146CF21-E405-3542-BA36-9745AB2C5B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E188D6EC-A463-2A43-AE37-35BEF3FDF995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="2360" windowWidth="30320" windowHeight="17120" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -1249,7 +1249,7 @@
   <dimension ref="A1:U71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="8" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U68" sqref="U68"/>
     </sheetView>
   </sheetViews>
@@ -3942,36 +3942,48 @@
       <c r="C57" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="D57" s="3" t="str">
+      <c r="D57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE)),"",VLOOKUP(RANK(E57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E57" s="1"/>
-      <c r="G57" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="E57" s="1">
+        <v>100</v>
+      </c>
+      <c r="G57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE)),"",VLOOKUP(RANK(H57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H57" s="1"/>
-      <c r="J57" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H57" s="1">
+        <v>60</v>
+      </c>
+      <c r="J57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE)),"",VLOOKUP(RANK(K57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K57" s="1"/>
-      <c r="M57" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K57" s="1">
+        <v>40</v>
+      </c>
+      <c r="M57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE)),"",VLOOKUP(RANK(N57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N57" s="1"/>
-      <c r="P57" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="N57" s="1">
+        <v>80</v>
+      </c>
+      <c r="P57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE)),"",VLOOKUP(RANK(Q57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q57" s="1"/>
-      <c r="S57" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>0</v>
+      </c>
+      <c r="S57" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE)),"",VLOOKUP(RANK(T57, ($T57,$Q57,$N57,$K57,$H57,$E57), 0),  $A$2:$C$7, $B57+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T57" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T57" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
@@ -3983,36 +3995,48 @@
       <c r="C58" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="D58" s="3" t="str">
+      <c r="D58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE)),"",VLOOKUP(RANK(E58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E58" s="1"/>
-      <c r="G58" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="E58" s="1">
+        <v>80</v>
+      </c>
+      <c r="G58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE)),"",VLOOKUP(RANK(H58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H58" s="1"/>
-      <c r="J58" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="H58" s="1">
+        <v>40</v>
+      </c>
+      <c r="J58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE)),"",VLOOKUP(RANK(K58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K58" s="1"/>
-      <c r="M58" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K58" s="1">
+        <v>20</v>
+      </c>
+      <c r="M58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE)),"",VLOOKUP(RANK(N58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N58" s="1"/>
-      <c r="P58" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="N58" s="1">
+        <v>60</v>
+      </c>
+      <c r="P58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE)),"",VLOOKUP(RANK(Q58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q58" s="1"/>
-      <c r="S58" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="1">
+        <v>0</v>
+      </c>
+      <c r="S58" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE)),"",VLOOKUP(RANK(T58, ($T58,$Q58,$N58,$K58,$H58,$E58), 0),  $A$2:$C$7, $B58+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T58" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="T58" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
@@ -4376,28 +4400,28 @@
       </c>
       <c r="E68" s="11">
         <f>SUM(D10:D65)</f>
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H68" s="11">
         <f>SUM(G10:G65)</f>
-        <v>-97.5</v>
+        <v>-127.5</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K68" s="11">
         <f>SUM(J10:J65)</f>
-        <v>-15</v>
+        <v>-60</v>
       </c>
       <c r="M68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N68" s="11">
         <f>SUM(M10:M65)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="P68" s="6" t="s">
         <v>12</v>
@@ -4411,7 +4435,7 @@
       </c>
       <c r="T68" s="11">
         <f>SUM(S10:S65)</f>
-        <v>-12.5</v>
+        <v>2.5</v>
       </c>
       <c r="U68" s="1">
         <f>SUM(E68,H68,K68,N68,Q68,T68)</f>

</xml_diff>

<commit_message>
Contest 50 DC vs CSK.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E188D6EC-A463-2A43-AE37-35BEF3FDF995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DDE917-4E64-6347-AD07-A7E3D3CBF2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="2360" windowWidth="30320" windowHeight="17120" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -605,157 +605,7 @@
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -4048,36 +3898,48 @@
       <c r="C59" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D59" s="3" t="str">
+      <c r="D59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE)),"",VLOOKUP(RANK(E59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E59" s="1"/>
-      <c r="G59" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E59" s="1">
+        <v>40</v>
+      </c>
+      <c r="G59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE)),"",VLOOKUP(RANK(H59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H59" s="1"/>
-      <c r="J59" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H59" s="1">
+        <v>60</v>
+      </c>
+      <c r="J59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE)),"",VLOOKUP(RANK(K59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K59" s="1"/>
-      <c r="M59" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="K59" s="1">
+        <v>80</v>
+      </c>
+      <c r="M59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE)),"",VLOOKUP(RANK(N59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N59" s="1"/>
-      <c r="P59" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="N59" s="1">
+        <v>100</v>
+      </c>
+      <c r="P59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE)),"",VLOOKUP(RANK(Q59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q59" s="1"/>
-      <c r="S59" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>0</v>
+      </c>
+      <c r="S59" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE)),"",VLOOKUP(RANK(T59, ($T59,$Q59,$N59,$K59,$H59,$E59), 0),  $A$2:$C$7, $B59+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T59" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T59" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
@@ -4400,28 +4262,28 @@
       </c>
       <c r="E68" s="11">
         <f>SUM(D10:D65)</f>
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H68" s="11">
         <f>SUM(G10:G65)</f>
-        <v>-127.5</v>
+        <v>-137.5</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K68" s="11">
         <f>SUM(J10:J65)</f>
-        <v>-60</v>
+        <v>-45</v>
       </c>
       <c r="M68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N68" s="11">
         <f>SUM(M10:M65)</f>
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="P68" s="6" t="s">
         <v>12</v>
@@ -4435,7 +4297,7 @@
       </c>
       <c r="T68" s="11">
         <f>SUM(S10:S65)</f>
-        <v>2.5</v>
+        <v>-22.5</v>
       </c>
       <c r="U68" s="1">
         <f>SUM(E68,H68,K68,N68,Q68,T68)</f>
@@ -4474,24 +4336,24 @@
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
   <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="32" priority="106" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="106" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="107" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="108" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68">
-    <cfRule type="cellIs" dxfId="29" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Contest 51 RR vs MI.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DDE917-4E64-6347-AD07-A7E3D3CBF2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE9ACDE-F766-D747-97F3-CDF99B1D9DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="2360" windowWidth="30320" windowHeight="17120" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -3951,36 +3951,48 @@
       <c r="C60" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D60" s="3" t="str">
+      <c r="D60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE)),"",VLOOKUP(RANK(E60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E60" s="1"/>
-      <c r="G60" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="E60" s="1">
+        <v>40</v>
+      </c>
+      <c r="G60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE)),"",VLOOKUP(RANK(H60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H60" s="1"/>
-      <c r="J60" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H60" s="1">
+        <v>20</v>
+      </c>
+      <c r="J60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE)),"",VLOOKUP(RANK(K60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K60" s="1"/>
-      <c r="M60" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="K60" s="1">
+        <v>80</v>
+      </c>
+      <c r="M60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE)),"",VLOOKUP(RANK(N60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N60" s="1"/>
-      <c r="P60" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="N60" s="1">
+        <v>100</v>
+      </c>
+      <c r="P60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE)),"",VLOOKUP(RANK(Q60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q60" s="1"/>
-      <c r="S60" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>0</v>
+      </c>
+      <c r="S60" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE)),"",VLOOKUP(RANK(T60, ($T60,$Q60,$N60,$K60,$H60,$E60), 0),  $A$2:$C$7, $B60+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T60" s="1"/>
+        <v>-10</v>
+      </c>
+      <c r="T60" s="1">
+        <v>60</v>
+      </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
@@ -4262,28 +4274,28 @@
       </c>
       <c r="E68" s="11">
         <f>SUM(D10:D65)</f>
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H68" s="11">
         <f>SUM(G10:G65)</f>
-        <v>-137.5</v>
+        <v>-162.5</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K68" s="11">
         <f>SUM(J10:J65)</f>
-        <v>-45</v>
+        <v>-30</v>
       </c>
       <c r="M68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N68" s="11">
         <f>SUM(M10:M65)</f>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="P68" s="6" t="s">
         <v>12</v>
@@ -4297,7 +4309,7 @@
       </c>
       <c r="T68" s="11">
         <f>SUM(S10:S65)</f>
-        <v>-22.5</v>
+        <v>-32.5</v>
       </c>
       <c r="U68" s="1">
         <f>SUM(E68,H68,K68,N68,Q68,T68)</f>

</xml_diff>

<commit_message>
Contest 52 RCB vs SRH.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE9ACDE-F766-D747-97F3-CDF99B1D9DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D64EF6-1E77-674B-B06C-1918AF0DE800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="2360" windowWidth="30320" windowHeight="17120" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -4004,36 +4004,48 @@
       <c r="C61" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="D61" s="3" t="str">
+      <c r="D61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE)),"",VLOOKUP(RANK(E61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E61" s="1"/>
-      <c r="G61" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="E61" s="1">
+        <v>100</v>
+      </c>
+      <c r="G61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE)),"",VLOOKUP(RANK(H61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H61" s="1"/>
-      <c r="J61" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="H61" s="1">
+        <v>20</v>
+      </c>
+      <c r="J61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE)),"",VLOOKUP(RANK(K61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K61" s="1"/>
-      <c r="M61" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K61" s="1">
+        <v>60</v>
+      </c>
+      <c r="M61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE)),"",VLOOKUP(RANK(N61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N61" s="1"/>
-      <c r="P61" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N61" s="1">
+        <v>40</v>
+      </c>
+      <c r="P61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE)),"",VLOOKUP(RANK(Q61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q61" s="1"/>
-      <c r="S61" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="1">
+        <v>0</v>
+      </c>
+      <c r="S61" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE)),"",VLOOKUP(RANK(T61, ($T61,$Q61,$N61,$K61,$H61,$E61), 0),  $A$2:$C$7, $B61+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T61" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="T61" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
@@ -4274,28 +4286,28 @@
       </c>
       <c r="E68" s="11">
         <f>SUM(D10:D65)</f>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H68" s="11">
         <f>SUM(G10:G65)</f>
-        <v>-162.5</v>
+        <v>-187.5</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K68" s="11">
         <f>SUM(J10:J65)</f>
-        <v>-30</v>
+        <v>-40</v>
       </c>
       <c r="M68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N68" s="11">
         <f>SUM(M10:M65)</f>
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="P68" s="6" t="s">
         <v>12</v>
@@ -4309,7 +4321,7 @@
       </c>
       <c r="T68" s="11">
         <f>SUM(S10:S65)</f>
-        <v>-32.5</v>
+        <v>-17.5</v>
       </c>
       <c r="U68" s="1">
         <f>SUM(E68,H68,K68,N68,Q68,T68)</f>

</xml_diff>

<commit_message>
Contest 53 CSK vs PBKS & Contest 54 KKR vs RR.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D64EF6-1E77-674B-B06C-1918AF0DE800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70256E6C-63C5-FE40-9246-7F2A1A351F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="2360" windowWidth="30320" windowHeight="17120" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -4057,36 +4057,46 @@
       <c r="C62" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D62" s="3" t="str">
+      <c r="D62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE)),"",VLOOKUP(RANK(E62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E62" s="1"/>
-      <c r="G62" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="E62" s="1">
+        <v>80</v>
+      </c>
+      <c r="G62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE)),"",VLOOKUP(RANK(H62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H62" s="1"/>
-      <c r="J62" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="H62" s="1">
+        <v>100</v>
+      </c>
+      <c r="J62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE)),"",VLOOKUP(RANK(K62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K62" s="1"/>
-      <c r="M62" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE)),"",VLOOKUP(RANK(N62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N62" s="1"/>
-      <c r="P62" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="K62" s="1">
+        <v>60</v>
+      </c>
+      <c r="M62" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="N62" s="1">
+        <v>40</v>
+      </c>
+      <c r="P62" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE)),"",VLOOKUP(RANK(Q62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q62" s="1"/>
-      <c r="S62" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE)),"",VLOOKUP(RANK(T62, ($T62,$Q62,$N62,$K62,$H62,$E62), 0),  $A$2:$C$7, $B62+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T62" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>0</v>
+      </c>
+      <c r="S62" s="3">
+        <v>-22.5</v>
+      </c>
+      <c r="T62" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -4098,36 +4108,48 @@
       <c r="C63" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="D63" s="3" t="str">
+      <c r="D63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE)),"",VLOOKUP(RANK(E63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E63" s="1"/>
-      <c r="G63" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="E63" s="1">
+        <v>80</v>
+      </c>
+      <c r="G63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE)),"",VLOOKUP(RANK(H63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H63" s="1"/>
-      <c r="J63" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H63" s="1">
+        <v>60</v>
+      </c>
+      <c r="J63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE)),"",VLOOKUP(RANK(K63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K63" s="1"/>
-      <c r="M63" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="K63" s="1">
+        <v>100</v>
+      </c>
+      <c r="M63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE)),"",VLOOKUP(RANK(N63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N63" s="1"/>
-      <c r="P63" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N63" s="1">
+        <v>40</v>
+      </c>
+      <c r="P63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE)),"",VLOOKUP(RANK(Q63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q63" s="1"/>
-      <c r="S63" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>0</v>
+      </c>
+      <c r="S63" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE)),"",VLOOKUP(RANK(T63, ($T63,$Q63,$N63,$K63,$H63,$E63), 0),  $A$2:$C$7, $B63+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T63" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T63" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
@@ -4286,28 +4308,28 @@
       </c>
       <c r="E68" s="11">
         <f>SUM(D10:D65)</f>
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H68" s="11">
         <f>SUM(G10:G65)</f>
-        <v>-187.5</v>
+        <v>-157.5</v>
       </c>
       <c r="J68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K68" s="11">
         <f>SUM(J10:J65)</f>
-        <v>-40</v>
+        <v>-10</v>
       </c>
       <c r="M68" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N68" s="11">
         <f>SUM(M10:M65)</f>
-        <v>70</v>
+        <v>27.5</v>
       </c>
       <c r="P68" s="6" t="s">
         <v>12</v>
@@ -4321,7 +4343,7 @@
       </c>
       <c r="T68" s="11">
         <f>SUM(S10:S65)</f>
-        <v>-17.5</v>
+        <v>-65</v>
       </c>
       <c r="U68" s="1">
         <f>SUM(E68,H68,K68,N68,Q68,T68)</f>

</xml_diff>

<commit_message>
Contest 55 SRH vs MI & Contest 56 RCB vs DC.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70256E6C-63C5-FE40-9246-7F2A1A351F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD4F31C-78DC-D94B-BC72-78507A9BD0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2500" yWindow="2360" windowWidth="30320" windowHeight="17120" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="102">
   <si>
     <t>Points</t>
   </si>
@@ -326,6 +326,18 @@
   </si>
   <si>
     <t>RCB vs DC</t>
+  </si>
+  <si>
+    <t>Qualifier 1</t>
+  </si>
+  <si>
+    <t>Eliminator</t>
+  </si>
+  <si>
+    <t>Qualifier 2</t>
+  </si>
+  <si>
+    <t>Finals</t>
   </si>
 </sst>
 </file>
@@ -605,7 +617,157 @@
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1096,11 +1258,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
-  <dimension ref="A1:U71"/>
+  <dimension ref="A1:U75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U68" sqref="U68"/>
+      <pane ySplit="8" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U72" sqref="U72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4161,36 +4323,48 @@
       <c r="C64" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="D64" s="3" t="str">
+      <c r="D64" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE)),"",VLOOKUP(RANK(E64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E64" s="1"/>
-      <c r="G64" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="E64" s="1">
+        <v>60</v>
+      </c>
+      <c r="G64" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE)),"",VLOOKUP(RANK(H64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H64" s="1"/>
-      <c r="J64" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="H64" s="1">
+        <v>80</v>
+      </c>
+      <c r="J64" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE)),"",VLOOKUP(RANK(K64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K64" s="1"/>
-      <c r="M64" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="K64" s="1">
+        <v>40</v>
+      </c>
+      <c r="M64" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE)),"",VLOOKUP(RANK(N64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N64" s="1"/>
-      <c r="P64" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="N64" s="1">
+        <v>100</v>
+      </c>
+      <c r="P64" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE)),"",VLOOKUP(RANK(Q64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q64" s="1"/>
-      <c r="S64" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>0</v>
+      </c>
+      <c r="S64" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE)),"",VLOOKUP(RANK(T64, ($T64,$Q64,$N64,$K64,$H64,$E64), 0),  $A$2:$C$7, $B64+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T64" s="1"/>
+        <v>-25</v>
+      </c>
+      <c r="T64" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
@@ -4202,174 +4376,346 @@
       <c r="C65" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="D65" s="3" t="str">
+      <c r="D65" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(E65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+        <v>15</v>
+      </c>
+      <c r="E65" s="1">
+        <v>80</v>
+      </c>
+      <c r="G65" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(H65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(H65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+        <v>-20</v>
+      </c>
+      <c r="H65" s="1">
+        <v>40</v>
+      </c>
+      <c r="J65" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(K65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(K65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+        <v>-10</v>
+      </c>
+      <c r="K65" s="1">
+        <v>60</v>
+      </c>
+      <c r="M65" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(N65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(N65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+        <v>-25</v>
+      </c>
+      <c r="N65" s="1">
+        <v>20</v>
+      </c>
+      <c r="P65" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(Q65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+        <v>0</v>
+      </c>
+      <c r="Q65" s="1">
+        <v>0</v>
+      </c>
+      <c r="S65" s="3">
+        <f>IF(ISERROR(VLOOKUP(RANK(T65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(T65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+        <v>40</v>
+      </c>
+      <c r="T65" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B66" s="1">
+        <v>2</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D66" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$C$7, $B66+1, FALSE)),"",VLOOKUP(RANK(E66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$C$7, $B66+1, FALSE))</f>
         <v/>
       </c>
-      <c r="E65" s="1"/>
-      <c r="G65" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(H65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(H65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+      <c r="E66" s="1"/>
+      <c r="G66" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$C$7, $B66+1, FALSE)),"",VLOOKUP(RANK(H66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$C$7, $B66+1, FALSE))</f>
         <v/>
       </c>
-      <c r="H65" s="1"/>
-      <c r="J65" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(K65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(K65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+      <c r="H66" s="1"/>
+      <c r="J66" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$C$7, $B66+1, FALSE)),"",VLOOKUP(RANK(K66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$C$7, $B66+1, FALSE))</f>
         <v/>
       </c>
-      <c r="K65" s="1"/>
-      <c r="M65" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(N65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(N65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+      <c r="K66" s="1"/>
+      <c r="M66" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$C$7, $B66+1, FALSE)),"",VLOOKUP(RANK(N66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$C$7, $B66+1, FALSE))</f>
         <v/>
       </c>
-      <c r="N65" s="1"/>
-      <c r="P65" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(Q65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(Q65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+      <c r="N66" s="1"/>
+      <c r="P66" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$C$7, $B66+1, FALSE)),"",VLOOKUP(RANK(Q66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$C$7, $B66+1, FALSE))</f>
         <v/>
       </c>
-      <c r="Q65" s="1"/>
-      <c r="S65" s="3" t="str">
-        <f>IF(ISERROR(VLOOKUP(RANK(T65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE)),"",VLOOKUP(RANK(T65, ($T65,$Q65,$N65,$K65,$H65,$E65), 0),  $A$2:$C$7, $B65+1, FALSE))</f>
+      <c r="Q66" s="1"/>
+      <c r="S66" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$C$7, $B66+1, FALSE)),"",VLOOKUP(RANK(T66, ($T66,$Q66,$N66,$K66,$H66,$E66), 0),  $A$2:$C$7, $B66+1, FALSE))</f>
         <v/>
       </c>
-      <c r="T65" s="1"/>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A66" s="5"/>
-      <c r="B66" s="1" t="s">
+      <c r="T66" s="1"/>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A67" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" s="1">
+        <v>2</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D67" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE)),"",VLOOKUP(RANK(E67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E67" s="1"/>
+      <c r="G67" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE)),"",VLOOKUP(RANK(H67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H67" s="1"/>
+      <c r="J67" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE)),"",VLOOKUP(RANK(K67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K67" s="1"/>
+      <c r="M67" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE)),"",VLOOKUP(RANK(N67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N67" s="1"/>
+      <c r="P67" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE)),"",VLOOKUP(RANK(Q67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q67" s="1"/>
+      <c r="S67" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE)),"",VLOOKUP(RANK(T67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T67" s="1"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B68" s="1">
+        <v>2</v>
+      </c>
+      <c r="C68" s="20"/>
+      <c r="D68" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE)),"",VLOOKUP(RANK(E68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E68" s="1"/>
+      <c r="G68" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE)),"",VLOOKUP(RANK(H68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H68" s="1"/>
+      <c r="J68" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE)),"",VLOOKUP(RANK(K68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K68" s="1"/>
+      <c r="M68" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE)),"",VLOOKUP(RANK(N68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N68" s="1"/>
+      <c r="P68" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE)),"",VLOOKUP(RANK(Q68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q68" s="1"/>
+      <c r="S68" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE)),"",VLOOKUP(RANK(T68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T68" s="1"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A69" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69" s="1">
+        <v>2</v>
+      </c>
+      <c r="C69" s="20"/>
+      <c r="D69" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(E69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE)),"",VLOOKUP(RANK(E69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="E69" s="1"/>
+      <c r="G69" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(H69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE)),"",VLOOKUP(RANK(H69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="H69" s="1"/>
+      <c r="J69" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(K69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE)),"",VLOOKUP(RANK(K69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="K69" s="1"/>
+      <c r="M69" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(N69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE)),"",VLOOKUP(RANK(N69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="N69" s="1"/>
+      <c r="P69" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(Q69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE)),"",VLOOKUP(RANK(Q69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="Q69" s="1"/>
+      <c r="S69" s="3" t="str">
+        <f>IF(ISERROR(VLOOKUP(RANK(T69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE)),"",VLOOKUP(RANK(T69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE))</f>
+        <v/>
+      </c>
+      <c r="T69" s="1"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A70" s="5"/>
+      <c r="B70" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C66" s="9"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="8" t="s">
+      <c r="C70" s="9"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G66" s="1"/>
-      <c r="H66" s="8" t="s">
+      <c r="G70" s="1"/>
+      <c r="H70" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J66" s="1"/>
-      <c r="K66" s="8" t="s">
+      <c r="J70" s="1"/>
+      <c r="K70" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M66" s="1"/>
-      <c r="N66" s="8" t="s">
+      <c r="M70" s="1"/>
+      <c r="N70" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="8" t="s">
+      <c r="P70" s="1"/>
+      <c r="Q70" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="S66" s="1"/>
-      <c r="T66" s="8" t="s">
+      <c r="S70" s="1"/>
+      <c r="T70" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="10" t="str">
-        <f>D9</f>
-        <v>Anantha</v>
-      </c>
-      <c r="G67" s="1"/>
-      <c r="H67" s="10" t="str">
-        <f>G9</f>
-        <v>Jayanth</v>
-      </c>
-      <c r="J67" s="1"/>
-      <c r="K67" s="10" t="str">
-        <f>J9</f>
-        <v>Justin</v>
-      </c>
-      <c r="M67" s="1"/>
-      <c r="N67" s="10" t="str">
-        <f>M9</f>
-        <v>Rapaka</v>
-      </c>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="10" t="str">
-        <f>P9</f>
-        <v>Sushma</v>
-      </c>
-      <c r="S67" s="1"/>
-      <c r="T67" s="10" t="str">
-        <f>S9</f>
-        <v>Sampath M</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21" ht="21" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E68" s="11">
-        <f>SUM(D10:D65)</f>
-        <v>120</v>
-      </c>
-      <c r="G68" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H68" s="11">
-        <f>SUM(G10:G65)</f>
-        <v>-157.5</v>
-      </c>
-      <c r="J68" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K68" s="11">
-        <f>SUM(J10:J65)</f>
-        <v>-10</v>
-      </c>
-      <c r="M68" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N68" s="11">
-        <f>SUM(M10:M65)</f>
-        <v>27.5</v>
-      </c>
-      <c r="P68" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q68" s="11">
-        <f>SUM(P10:P65)</f>
-        <v>85</v>
-      </c>
-      <c r="S68" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="T68" s="11">
-        <f>SUM(S10:S65)</f>
-        <v>-65</v>
-      </c>
-      <c r="U68" s="1">
-        <f>SUM(E68,H68,K68,N68,Q68,T68)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="10" t="str">
+        <f>D9</f>
+        <v>Anantha</v>
+      </c>
+      <c r="G71" s="1"/>
+      <c r="H71" s="10" t="str">
+        <f>G9</f>
+        <v>Jayanth</v>
+      </c>
+      <c r="J71" s="1"/>
+      <c r="K71" s="10" t="str">
+        <f>J9</f>
+        <v>Justin</v>
+      </c>
+      <c r="M71" s="1"/>
+      <c r="N71" s="10" t="str">
+        <f>M9</f>
+        <v>Rapaka</v>
+      </c>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="10" t="str">
+        <f>P9</f>
+        <v>Sushma</v>
+      </c>
+      <c r="S71" s="1"/>
+      <c r="T71" s="10" t="str">
+        <f>S9</f>
+        <v>Sampath M</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72" s="11">
+        <f>SUM(D10:D69)</f>
+        <v>125</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H72" s="11">
+        <f>SUM(G10:G69)</f>
+        <v>-162.5</v>
+      </c>
+      <c r="J72" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K72" s="11">
+        <f>SUM(J10:J69)</f>
+        <v>-40</v>
+      </c>
+      <c r="M72" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N72" s="11">
+        <f>SUM(M10:M69)</f>
+        <v>42.5</v>
+      </c>
+      <c r="P72" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q72" s="11">
+        <f>SUM(P10:P69)</f>
+        <v>85</v>
+      </c>
+      <c r="S72" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="T72" s="11">
+        <f>SUM(S10:S69)</f>
+        <v>-50</v>
+      </c>
+      <c r="U72" s="1">
+        <f>SUM(E72,H72,K72,N72,Q72,T72)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4381,18 +4727,18 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="17" priority="106" operator="lessThan">
+  <conditionalFormatting sqref="E72">
+    <cfRule type="cellIs" dxfId="32" priority="121" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="122" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="123" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H68">
+  <conditionalFormatting sqref="H72">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -4403,7 +4749,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
+  <conditionalFormatting sqref="K72">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -4414,7 +4760,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N68">
+  <conditionalFormatting sqref="N72">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -4425,7 +4771,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q68">
+  <conditionalFormatting sqref="Q72">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -4436,7 +4782,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T68">
+  <conditionalFormatting sqref="T72">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Qualifier 2 DC vs KKR.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDE98F4-BAFB-2643-B184-0E36DCD14E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3DF7A3-3EE2-B94A-8B98-92BAFDE25FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="2260" windowWidth="30820" windowHeight="17540" activeTab="1" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="1640" yWindow="2260" windowWidth="30820" windowHeight="17540" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="102">
   <si>
     <t>Points</t>
   </si>
@@ -1251,7 +1251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
   <dimension ref="A1:U86"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q86" sqref="Q86"/>
     </sheetView>
@@ -4501,11 +4501,13 @@
       <c r="N67" s="1">
         <v>40</v>
       </c>
-      <c r="P67" s="3" t="str">
+      <c r="P67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE)),"",VLOOKUP(RANK(Q67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q67" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q67" s="1">
+        <v>0</v>
+      </c>
       <c r="S67" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE)),"",VLOOKUP(RANK(T67, ($T67,$Q67,$N67,$K67,$H67,$E67), 0),  $A$2:$C$7, $B67+1, FALSE))</f>
         <v>-10</v>
@@ -4521,37 +4523,51 @@
       <c r="B68" s="1">
         <v>2</v>
       </c>
-      <c r="C68" s="15"/>
-      <c r="D68" s="3" t="str">
+      <c r="C68" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE)),"",VLOOKUP(RANK(E68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E68" s="1"/>
-      <c r="G68" s="3" t="str">
+        <v>15</v>
+      </c>
+      <c r="E68" s="1">
+        <v>80</v>
+      </c>
+      <c r="G68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE)),"",VLOOKUP(RANK(H68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H68" s="1"/>
-      <c r="J68" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H68" s="1">
+        <v>60</v>
+      </c>
+      <c r="J68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE)),"",VLOOKUP(RANK(K68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K68" s="1"/>
-      <c r="M68" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K68" s="1">
+        <v>20</v>
+      </c>
+      <c r="M68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE)),"",VLOOKUP(RANK(N68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N68" s="1"/>
-      <c r="P68" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="N68" s="1">
+        <v>100</v>
+      </c>
+      <c r="P68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE)),"",VLOOKUP(RANK(Q68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q68" s="1"/>
-      <c r="S68" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="1">
+        <v>0</v>
+      </c>
+      <c r="S68" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE)),"",VLOOKUP(RANK(T68, ($T68,$Q68,$N68,$K68,$H68,$E68), 0),  $A$2:$C$7, $B68+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T68" s="1"/>
+        <v>-20</v>
+      </c>
+      <c r="T68" s="1">
+        <v>40</v>
+      </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
@@ -4667,28 +4683,28 @@
       </c>
       <c r="E72" s="11">
         <f>SUM(D10:D69)</f>
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="G72" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H72" s="11">
         <f>SUM(G10:G69)</f>
-        <v>-147.5</v>
+        <v>-157.5</v>
       </c>
       <c r="J72" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K72" s="11">
         <f>SUM(J10:J69)</f>
-        <v>-50</v>
+        <v>-75</v>
       </c>
       <c r="M72" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N72" s="11">
         <f>SUM(M10:M69)</f>
-        <v>62.5</v>
+        <v>102.5</v>
       </c>
       <c r="P72" s="6" t="s">
         <v>12</v>
@@ -4702,7 +4718,7 @@
       </c>
       <c r="T72" s="11">
         <f>SUM(S10:S69)</f>
-        <v>-80</v>
+        <v>-100</v>
       </c>
       <c r="U72" s="1">
         <f>SUM(E72,H72,K72,N72,Q72,T72)</f>
@@ -4794,33 +4810,35 @@
       <c r="D80" s="1">
         <v>11</v>
       </c>
-      <c r="E80" s="1"/>
+      <c r="E80" s="1">
+        <v>5</v>
+      </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1">
         <f>SUM(C80:F80)</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="L80" s="26" t="s">
         <v>5</v>
       </c>
       <c r="M80" s="11">
         <f>E72</f>
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="N80" s="29">
         <v>-200</v>
       </c>
       <c r="O80" s="11">
         <f>G80</f>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="P80" s="11">
         <f>IFERROR((-SUM($N$80:$N$85)/SUM($O$80:$O$85))*O80, 0)</f>
-        <v>571.42857142857144</v>
+        <v>460.67415730337081</v>
       </c>
       <c r="Q80" s="11">
         <f>SUM(M80,N80,P80)</f>
-        <v>501.42857142857144</v>
+        <v>405.67415730337081</v>
       </c>
       <c r="R80" s="26" t="s">
         <v>5</v>
@@ -4836,33 +4854,35 @@
       <c r="D81" s="1">
         <v>3</v>
       </c>
-      <c r="E81" s="1"/>
+      <c r="E81" s="1">
+        <v>7</v>
+      </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1">
         <f t="shared" ref="G81:G85" si="0">SUM(C81:F81)</f>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="L81" s="26" t="s">
         <v>6</v>
       </c>
       <c r="M81" s="11">
         <f>H72</f>
-        <v>-147.5</v>
+        <v>-157.5</v>
       </c>
       <c r="N81" s="29">
         <v>-200</v>
       </c>
       <c r="O81" s="11">
         <f t="shared" ref="O81:O85" si="1">G81</f>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="P81" s="11">
         <f t="shared" ref="P81:P85" si="2">IFERROR((-SUM($N$80:$N$85)/SUM($O$80:$O$85))*O81, 0)</f>
-        <v>222.22222222222223</v>
+        <v>235.95505617977528</v>
       </c>
       <c r="Q81" s="11">
         <f t="shared" ref="Q81:Q85" si="3">SUM(M81,N81,P81)</f>
-        <v>-125.27777777777777</v>
+        <v>-121.54494382022472</v>
       </c>
       <c r="R81" s="26" t="s">
         <v>6</v>
@@ -4878,7 +4898,9 @@
       <c r="D82" s="1">
         <v>5</v>
       </c>
-      <c r="E82" s="1"/>
+      <c r="E82" s="1">
+        <v>0</v>
+      </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1">
         <f t="shared" si="0"/>
@@ -4889,7 +4911,7 @@
       </c>
       <c r="M82" s="11">
         <f>K72</f>
-        <v>-50</v>
+        <v>-75</v>
       </c>
       <c r="N82" s="29">
         <v>-200</v>
@@ -4900,11 +4922,11 @@
       </c>
       <c r="P82" s="11">
         <f t="shared" si="2"/>
-        <v>79.365079365079367</v>
+        <v>56.17977528089888</v>
       </c>
       <c r="Q82" s="11">
         <f t="shared" si="3"/>
-        <v>-170.63492063492063</v>
+        <v>-218.82022471910113</v>
       </c>
       <c r="R82" s="26" t="s">
         <v>7</v>
@@ -4920,33 +4942,35 @@
       <c r="D83" s="1">
         <v>0</v>
       </c>
-      <c r="E83" s="1"/>
+      <c r="E83" s="1">
+        <v>3</v>
+      </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L83" s="26" t="s">
         <v>8</v>
       </c>
       <c r="M83" s="11">
         <f>N72</f>
-        <v>62.5</v>
+        <v>102.5</v>
       </c>
       <c r="N83" s="29">
         <v>-200</v>
       </c>
       <c r="O83" s="11">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P83" s="11">
         <f t="shared" si="2"/>
-        <v>47.61904761904762</v>
+        <v>67.415730337078656</v>
       </c>
       <c r="Q83" s="11">
         <f t="shared" si="3"/>
-        <v>-89.88095238095238</v>
+        <v>-30.084269662921344</v>
       </c>
       <c r="R83" s="26" t="s">
         <v>8</v>
@@ -5008,33 +5032,35 @@
       <c r="D85" s="1">
         <v>5</v>
       </c>
-      <c r="E85" s="1"/>
+      <c r="E85" s="1">
+        <v>11</v>
+      </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="L85" s="26" t="s">
         <v>10</v>
       </c>
       <c r="M85" s="11">
         <f>T72</f>
-        <v>-80</v>
+        <v>-100</v>
       </c>
       <c r="N85" s="29">
         <v>-200</v>
       </c>
       <c r="O85" s="11">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="P85" s="11">
         <f t="shared" si="2"/>
-        <v>79.365079365079367</v>
+        <v>179.77528089887642</v>
       </c>
       <c r="Q85" s="11">
         <f t="shared" si="3"/>
-        <v>-200.63492063492063</v>
+        <v>-120.22471910112358</v>
       </c>
       <c r="R85" s="26" t="s">
         <v>10</v>
@@ -5179,8 +5205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8336F3D9-B2DA-B14A-BEAC-3FAB2279E4CE}">
   <dimension ref="F19:K57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N46" sqref="N46"/>
+    <sheetView showGridLines="0" topLeftCell="C32" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5364,7 +5390,9 @@
       <c r="J44" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="K44" s="6"/>
+      <c r="K44" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="45" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F45" s="6" t="s">
@@ -5379,7 +5407,9 @@
       <c r="J45" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="K45" s="6"/>
+      <c r="K45" s="6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="46" spans="6:11" x14ac:dyDescent="0.2">
       <c r="F46" s="6" t="s">

</xml_diff>

<commit_message>
Finals CSK vs KKR.
</commit_message>
<xml_diff>
--- a/2021/AFA 2021.xlsx
+++ b/2021/AFA 2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkpaul/Personal/Things/IPL/2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3DF7A3-3EE2-B94A-8B98-92BAFDE25FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B95C1A-19A5-3441-9795-DAD758C7F68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="2260" windowWidth="30820" windowHeight="17540" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
+    <workbookView xWindow="1460" yWindow="2420" windowWidth="30820" windowHeight="17540" activeTab="1" xr2:uid="{7813E1F3-AD71-F349-B41B-B75E130580BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="104">
   <si>
     <t>Points</t>
   </si>
@@ -328,9 +328,6 @@
     <t>Qualifier 2 DC vs KKR</t>
   </si>
   <si>
-    <t xml:space="preserve">Finals CSK vs </t>
-  </si>
-  <si>
     <t>Rank 1</t>
   </si>
   <si>
@@ -338,6 +335,15 @@
   </si>
   <si>
     <t>Jayantha</t>
+  </si>
+  <si>
+    <t>Finals CSK vs KKR</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Congrats</t>
   </si>
 </sst>
 </file>
@@ -573,7 +579,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -632,13 +638,136 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1251,9 +1380,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BE9CB7-B9A7-B347-86F0-C3EB9B5BFBBD}">
   <dimension ref="A1:U86"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q86" sqref="Q86"/>
+      <selection pane="bottomLeft" activeCell="Q80" sqref="Q80:R85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4576,37 +4705,51 @@
       <c r="B69" s="1">
         <v>2</v>
       </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="3" t="str">
+      <c r="C69" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(E69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE)),"",VLOOKUP(RANK(E69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="E69" s="1"/>
-      <c r="G69" s="3" t="str">
+        <v>40</v>
+      </c>
+      <c r="E69" s="1">
+        <v>100</v>
+      </c>
+      <c r="G69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(H69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE)),"",VLOOKUP(RANK(H69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="H69" s="1"/>
-      <c r="J69" s="3" t="str">
+        <v>-10</v>
+      </c>
+      <c r="H69" s="1">
+        <v>60</v>
+      </c>
+      <c r="J69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(K69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE)),"",VLOOKUP(RANK(K69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="K69" s="1"/>
-      <c r="M69" s="3" t="str">
+        <v>-25</v>
+      </c>
+      <c r="K69" s="1">
+        <v>20</v>
+      </c>
+      <c r="M69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(N69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE)),"",VLOOKUP(RANK(N69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="N69" s="1"/>
-      <c r="P69" s="3" t="str">
+        <v>-20</v>
+      </c>
+      <c r="N69" s="1">
+        <v>40</v>
+      </c>
+      <c r="P69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(Q69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE)),"",VLOOKUP(RANK(Q69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="Q69" s="1"/>
-      <c r="S69" s="3" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="1">
+        <v>0</v>
+      </c>
+      <c r="S69" s="3">
         <f>IF(ISERROR(VLOOKUP(RANK(T69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE)),"",VLOOKUP(RANK(T69, ($T69,$Q69,$N69,$K69,$H69,$E69), 0),  $A$2:$C$7, $B69+1, FALSE))</f>
-        <v/>
-      </c>
-      <c r="T69" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="T69" s="1">
+        <v>80</v>
+      </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="5"/>
@@ -4683,28 +4826,28 @@
       </c>
       <c r="E72" s="11">
         <f>SUM(D10:D69)</f>
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="G72" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H72" s="11">
         <f>SUM(G10:G69)</f>
-        <v>-157.5</v>
+        <v>-167.5</v>
       </c>
       <c r="J72" s="6" t="s">
         <v>12</v>
       </c>
       <c r="K72" s="11">
         <f>SUM(J10:J69)</f>
-        <v>-75</v>
+        <v>-100</v>
       </c>
       <c r="M72" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N72" s="11">
         <f>SUM(M10:M69)</f>
-        <v>102.5</v>
+        <v>82.5</v>
       </c>
       <c r="P72" s="6" t="s">
         <v>12</v>
@@ -4718,7 +4861,7 @@
       </c>
       <c r="T72" s="11">
         <f>SUM(S10:S69)</f>
-        <v>-100</v>
+        <v>-85</v>
       </c>
       <c r="U72" s="1">
         <f>SUM(E72,H72,K72,N72,Q72,T72)</f>
@@ -4813,32 +4956,34 @@
       <c r="E80" s="1">
         <v>5</v>
       </c>
-      <c r="F80" s="1"/>
+      <c r="F80" s="1">
+        <v>3</v>
+      </c>
       <c r="G80" s="1">
         <f>SUM(C80:F80)</f>
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="L80" s="26" t="s">
         <v>5</v>
       </c>
       <c r="M80" s="11">
         <f>E72</f>
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="N80" s="29">
         <v>-200</v>
       </c>
       <c r="O80" s="11">
         <f>G80</f>
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="P80" s="11">
         <f>IFERROR((-SUM($N$80:$N$85)/SUM($O$80:$O$85))*O80, 0)</f>
-        <v>460.67415730337081</v>
+        <v>343.75</v>
       </c>
       <c r="Q80" s="11">
         <f>SUM(M80,N80,P80)</f>
-        <v>405.67415730337081</v>
+        <v>328.75</v>
       </c>
       <c r="R80" s="26" t="s">
         <v>5</v>
@@ -4857,32 +5002,34 @@
       <c r="E81" s="1">
         <v>7</v>
       </c>
-      <c r="F81" s="1"/>
+      <c r="F81" s="1">
+        <v>11</v>
+      </c>
       <c r="G81" s="1">
         <f t="shared" ref="G81:G85" si="0">SUM(C81:F81)</f>
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="L81" s="26" t="s">
         <v>6</v>
       </c>
       <c r="M81" s="11">
         <f>H72</f>
-        <v>-157.5</v>
+        <v>-167.5</v>
       </c>
       <c r="N81" s="29">
         <v>-200</v>
       </c>
       <c r="O81" s="11">
         <f t="shared" ref="O81:O85" si="1">G81</f>
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="P81" s="11">
         <f t="shared" ref="P81:P85" si="2">IFERROR((-SUM($N$80:$N$85)/SUM($O$80:$O$85))*O81, 0)</f>
-        <v>235.95505617977528</v>
+        <v>250</v>
       </c>
       <c r="Q81" s="11">
         <f t="shared" ref="Q81:Q85" si="3">SUM(M81,N81,P81)</f>
-        <v>-121.54494382022472</v>
+        <v>-117.5</v>
       </c>
       <c r="R81" s="26" t="s">
         <v>6</v>
@@ -4901,32 +5048,34 @@
       <c r="E82" s="1">
         <v>0</v>
       </c>
-      <c r="F82" s="1"/>
+      <c r="F82" s="1">
+        <v>3</v>
+      </c>
       <c r="G82" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L82" s="26" t="s">
         <v>7</v>
       </c>
       <c r="M82" s="11">
         <f>K72</f>
-        <v>-75</v>
+        <v>-100</v>
       </c>
       <c r="N82" s="29">
         <v>-200</v>
       </c>
       <c r="O82" s="11">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="P82" s="11">
         <f t="shared" si="2"/>
-        <v>56.17977528089888</v>
+        <v>62.5</v>
       </c>
       <c r="Q82" s="11">
         <f t="shared" si="3"/>
-        <v>-218.82022471910113</v>
+        <v>-237.5</v>
       </c>
       <c r="R82" s="26" t="s">
         <v>7</v>
@@ -4945,32 +5094,34 @@
       <c r="E83" s="1">
         <v>3</v>
       </c>
-      <c r="F83" s="1"/>
+      <c r="F83" s="1">
+        <v>11</v>
+      </c>
       <c r="G83" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="L83" s="26" t="s">
         <v>8</v>
       </c>
       <c r="M83" s="11">
         <f>N72</f>
-        <v>102.5</v>
+        <v>82.5</v>
       </c>
       <c r="N83" s="29">
         <v>-200</v>
       </c>
       <c r="O83" s="11">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="P83" s="11">
         <f t="shared" si="2"/>
-        <v>67.415730337078656</v>
+        <v>132.8125</v>
       </c>
       <c r="Q83" s="11">
         <f t="shared" si="3"/>
-        <v>-30.084269662921344</v>
+        <v>15.3125</v>
       </c>
       <c r="R83" s="26" t="s">
         <v>8</v>
@@ -5035,32 +5186,34 @@
       <c r="E85" s="1">
         <v>11</v>
       </c>
-      <c r="F85" s="1"/>
+      <c r="F85" s="1">
+        <v>11</v>
+      </c>
       <c r="G85" s="1">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="L85" s="26" t="s">
         <v>10</v>
       </c>
       <c r="M85" s="11">
         <f>T72</f>
-        <v>-100</v>
+        <v>-85</v>
       </c>
       <c r="N85" s="29">
         <v>-200</v>
       </c>
       <c r="O85" s="11">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="P85" s="11">
         <f t="shared" si="2"/>
-        <v>179.77528089887642</v>
+        <v>210.9375</v>
       </c>
       <c r="Q85" s="11">
         <f t="shared" si="3"/>
-        <v>-120.22471910112358</v>
+        <v>-74.0625</v>
       </c>
       <c r="R85" s="26" t="s">
         <v>10</v>
@@ -5088,94 +5241,593 @@
     <mergeCell ref="P8:Q8"/>
   </mergeCells>
   <conditionalFormatting sqref="E72">
-    <cfRule type="cellIs" dxfId="29" priority="133" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="133" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="134" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="135" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="135" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T72">
-    <cfRule type="cellIs" dxfId="26" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H72">
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="25" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="27" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K72">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="22" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="24" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N72">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="19" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="21" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q72">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M80:M84">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q80:Q84">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M85">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q85">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8336F3D9-B2DA-B14A-BEAC-3FAB2279E4CE}">
+  <dimension ref="F19:N71"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F45" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P67" sqref="P67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="19" spans="6:11" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="6:11" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="6:11" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F27" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F36" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F38" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F40" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F44" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F45" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F46" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F47" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F48" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F49" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F52" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H52" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F53" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J53" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F54" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H54" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F55" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H55" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F56" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="F57" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H57" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="6:13" x14ac:dyDescent="0.2">
+      <c r="J60" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K60" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="L60" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="6:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="J61" s="1">
+        <v>1</v>
+      </c>
+      <c r="K61" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="L61" s="11">
+        <v>328.75</v>
+      </c>
+      <c r="M61" s="30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="6:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="J62" s="1">
+        <v>2</v>
+      </c>
+      <c r="K62" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="L62" s="11">
+        <v>85</v>
+      </c>
+      <c r="M62" s="30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="6:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="J63" s="1">
+        <v>3</v>
+      </c>
+      <c r="K63" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="L63" s="11">
+        <v>15.3125</v>
+      </c>
+      <c r="M63" s="30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="64" spans="6:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="J64" s="1">
+        <v>4</v>
+      </c>
+      <c r="K64" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="L64" s="11">
+        <v>-74.0625</v>
+      </c>
+    </row>
+    <row r="65" spans="9:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="J65" s="1">
+        <v>5</v>
+      </c>
+      <c r="K65" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L65" s="11">
+        <v>-117.5</v>
+      </c>
+    </row>
+    <row r="66" spans="9:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="J66" s="1">
+        <v>6</v>
+      </c>
+      <c r="K66" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="L66" s="11">
+        <v>-237.5</v>
+      </c>
+    </row>
+    <row r="67" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+    </row>
+    <row r="68" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="4"/>
+    </row>
+    <row r="69" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+    </row>
+    <row r="70" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+    </row>
+    <row r="71" spans="9:14" x14ac:dyDescent="0.2">
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J61:L66">
+    <sortCondition descending="1" ref="L61:L66"/>
+  </sortState>
+  <conditionalFormatting sqref="L66">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L61:L65">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -5186,322 +5838,6 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q85">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8336F3D9-B2DA-B14A-BEAC-3FAB2279E4CE}">
-  <dimension ref="F19:K57"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C32" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="19" spans="6:11" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="6:11" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="6:11" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F27" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F28" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F29" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F30" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F31" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F32" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F36" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J36" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="K36" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F37" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="H37" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="K37" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F38" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F39" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H39" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F40" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G40" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F41" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H41" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F44" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="K44" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F45" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H45" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F46" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H46" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F47" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H47" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F48" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G48" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H48" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F49" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H49" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F52" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H52" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="53" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F53" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-    </row>
-    <row r="54" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F54" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-    </row>
-    <row r="55" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F55" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-    </row>
-    <row r="56" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F56" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-    </row>
-    <row r="57" spans="6:8" x14ac:dyDescent="0.2">
-      <c r="F57" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>